<commit_message>
End of Day commit
</commit_message>
<xml_diff>
--- a/3. Scribbling/SamsaraExcel.xlsx
+++ b/3. Scribbling/SamsaraExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Drive\Writing Grand Compile\Repository\Project Samsara\Obsidian\ProjectSamsara\3. Scribbling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07083C44-3304-4A3E-9776-194E736597DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3CCD21-B58D-4ED1-9FC5-2AC0E635D0B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="300" windowWidth="23256" windowHeight="12804" activeTab="2" xr2:uid="{E6D84C89-D0D8-4C46-AF33-8B126112E9FD}"/>
+    <workbookView xWindow="6852" yWindow="2820" windowWidth="16188" windowHeight="9420" activeTab="2" xr2:uid="{E6D84C89-D0D8-4C46-AF33-8B126112E9FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Workshop" sheetId="13" r:id="rId1"/>
@@ -1241,7 +1241,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1914" uniqueCount="586">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1924" uniqueCount="596">
   <si>
     <t>Tier</t>
   </si>
@@ -3015,6 +3015,36 @@
   </si>
   <si>
     <t>Flechette 'Accelerator' Rifles</t>
+  </si>
+  <si>
+    <t>Referring To</t>
+  </si>
+  <si>
+    <t>Karahn</t>
+  </si>
+  <si>
+    <t>Zahiran</t>
+  </si>
+  <si>
+    <t>Adrian</t>
+  </si>
+  <si>
+    <t>Nefelian</t>
+  </si>
+  <si>
+    <t>Ciceran</t>
+  </si>
+  <si>
+    <t>Yurian</t>
+  </si>
+  <si>
+    <t>Ryian</t>
+  </si>
+  <si>
+    <t>Morrian</t>
+  </si>
+  <si>
+    <t>Leilan</t>
   </si>
 </sst>
 </file>
@@ -3536,7 +3566,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="321">
+  <cellXfs count="322">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4106,6 +4136,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4166,10 +4200,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4202,10 +4236,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13215,10 +13246,10 @@
       <c r="A19" t="s">
         <v>575</v>
       </c>
-      <c r="B19" s="319" t="s">
+      <c r="B19" s="287" t="s">
         <v>585</v>
       </c>
-      <c r="C19" s="320" t="s">
+      <c r="C19" s="288" t="s">
         <v>579</v>
       </c>
       <c r="D19" t="s">
@@ -13258,10 +13289,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A1" s="318" t="s">
+      <c r="A1" s="320" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="318"/>
+      <c r="B1" s="320"/>
       <c r="F1" t="s">
         <v>253</v>
       </c>
@@ -17932,29 +17963,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="287" t="s">
+      <c r="A1" s="289" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="288"/>
-      <c r="C1" s="288"/>
-      <c r="D1" s="289"/>
-      <c r="F1" s="290" t="s">
+      <c r="B1" s="290"/>
+      <c r="C1" s="290"/>
+      <c r="D1" s="291"/>
+      <c r="F1" s="292" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="290"/>
-      <c r="H1" s="290"/>
-      <c r="I1" s="290"/>
-      <c r="J1" s="290"/>
-      <c r="K1" s="290"/>
-      <c r="N1" s="287" t="s">
+      <c r="G1" s="292"/>
+      <c r="H1" s="292"/>
+      <c r="I1" s="292"/>
+      <c r="J1" s="292"/>
+      <c r="K1" s="292"/>
+      <c r="N1" s="289" t="s">
         <v>38</v>
       </c>
-      <c r="O1" s="291"/>
-      <c r="P1" s="291"/>
-      <c r="Q1" s="291"/>
-      <c r="R1" s="291"/>
-      <c r="S1" s="291"/>
-      <c r="T1" s="292"/>
+      <c r="O1" s="293"/>
+      <c r="P1" s="293"/>
+      <c r="Q1" s="293"/>
+      <c r="R1" s="293"/>
+      <c r="S1" s="293"/>
+      <c r="T1" s="294"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -18559,10 +18590,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7594C28-F5C4-4873-B2AF-F5CC5CA2F682}">
-  <dimension ref="A1:AC16"/>
+  <dimension ref="A1:AD16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="X19" sqref="X19"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="104" workbookViewId="0">
+      <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18574,78 +18605,80 @@
     <col min="6" max="6" width="18" customWidth="1"/>
     <col min="7" max="7" width="17.6640625" customWidth="1"/>
     <col min="18" max="18" width="3.44140625" customWidth="1"/>
-    <col min="19" max="20" width="16.33203125" customWidth="1"/>
-    <col min="21" max="21" width="18.109375" customWidth="1"/>
-    <col min="22" max="22" width="14.21875" customWidth="1"/>
-    <col min="23" max="23" width="21.109375" customWidth="1"/>
-    <col min="24" max="24" width="7.44140625" customWidth="1"/>
-    <col min="25" max="25" width="5.77734375" customWidth="1"/>
-    <col min="26" max="26" width="19.5546875" customWidth="1"/>
-    <col min="27" max="27" width="18.21875" customWidth="1"/>
-    <col min="28" max="28" width="19.5546875" customWidth="1"/>
-    <col min="29" max="29" width="21.44140625" customWidth="1"/>
+    <col min="19" max="21" width="16.33203125" customWidth="1"/>
+    <col min="22" max="22" width="18.109375" customWidth="1"/>
+    <col min="23" max="23" width="14.21875" customWidth="1"/>
+    <col min="24" max="24" width="21.109375" customWidth="1"/>
+    <col min="25" max="25" width="7.44140625" customWidth="1"/>
+    <col min="26" max="26" width="5.77734375" customWidth="1"/>
+    <col min="27" max="27" width="19.5546875" customWidth="1"/>
+    <col min="28" max="28" width="18.21875" customWidth="1"/>
+    <col min="29" max="29" width="19.5546875" customWidth="1"/>
+    <col min="30" max="30" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="293" t="s">
+    <row r="1" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="295" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="293"/>
-      <c r="C1" s="293"/>
-      <c r="D1" s="293"/>
-      <c r="E1" s="293"/>
-      <c r="F1" s="293"/>
-      <c r="G1" s="293"/>
-      <c r="H1" s="293"/>
-      <c r="I1" s="293"/>
-      <c r="J1" s="293"/>
-      <c r="K1" s="293"/>
-      <c r="L1" s="293"/>
-      <c r="M1" s="293"/>
-      <c r="N1" s="293"/>
-      <c r="R1" s="294" t="s">
+      <c r="B1" s="295"/>
+      <c r="C1" s="295"/>
+      <c r="D1" s="295"/>
+      <c r="E1" s="295"/>
+      <c r="F1" s="295"/>
+      <c r="G1" s="295"/>
+      <c r="H1" s="295"/>
+      <c r="I1" s="295"/>
+      <c r="J1" s="295"/>
+      <c r="K1" s="295"/>
+      <c r="L1" s="295"/>
+      <c r="M1" s="295"/>
+      <c r="N1" s="295"/>
+      <c r="R1" s="296" t="s">
         <v>488</v>
       </c>
-      <c r="S1" s="295"/>
-      <c r="T1" s="295"/>
-      <c r="U1" s="295"/>
-      <c r="V1" s="295"/>
-      <c r="W1" s="295"/>
-      <c r="X1" s="295"/>
-      <c r="Y1" s="295"/>
-      <c r="Z1" s="295"/>
-      <c r="AA1" s="295"/>
-      <c r="AB1" s="295"/>
-      <c r="AC1" s="296"/>
-    </row>
-    <row r="2" spans="1:29" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="293" t="s">
+      <c r="S1" s="297"/>
+      <c r="T1" s="297"/>
+      <c r="U1" s="297"/>
+      <c r="V1" s="297"/>
+      <c r="W1" s="297"/>
+      <c r="X1" s="297"/>
+      <c r="Y1" s="297"/>
+      <c r="Z1" s="297"/>
+      <c r="AA1" s="297"/>
+      <c r="AB1" s="297"/>
+      <c r="AC1" s="297"/>
+      <c r="AD1" s="298"/>
+    </row>
+    <row r="2" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J2" s="295" t="s">
         <v>423</v>
       </c>
-      <c r="K2" s="293"/>
-      <c r="L2" s="293"/>
-      <c r="M2" s="293"/>
-      <c r="N2" s="293"/>
-      <c r="R2" s="300" t="s">
+      <c r="K2" s="295"/>
+      <c r="L2" s="295"/>
+      <c r="M2" s="295"/>
+      <c r="N2" s="295"/>
+      <c r="R2" s="302" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="298" t="s">
+      <c r="S2" s="300" t="s">
         <v>525</v>
       </c>
-      <c r="T2" s="298"/>
-      <c r="U2" s="298"/>
-      <c r="V2" s="298"/>
-      <c r="W2" s="298"/>
-      <c r="X2" s="298"/>
-      <c r="Y2" s="299"/>
-      <c r="Z2" s="297" t="s">
+      <c r="T2" s="300"/>
+      <c r="U2" s="300"/>
+      <c r="V2" s="300"/>
+      <c r="W2" s="300"/>
+      <c r="X2" s="300"/>
+      <c r="Y2" s="300"/>
+      <c r="Z2" s="301"/>
+      <c r="AA2" s="299" t="s">
         <v>524</v>
       </c>
-      <c r="AA2" s="298"/>
-      <c r="AB2" s="298"/>
-      <c r="AC2" s="299"/>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="AB2" s="300"/>
+      <c r="AC2" s="300"/>
+      <c r="AD2" s="301"/>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -18682,7 +18715,7 @@
       <c r="N3" s="233">
         <v>5</v>
       </c>
-      <c r="R3" s="301"/>
+      <c r="R3" s="303"/>
       <c r="S3" s="284" t="s">
         <v>2</v>
       </c>
@@ -18690,34 +18723,37 @@
         <v>549</v>
       </c>
       <c r="U3" s="255" t="s">
+        <v>586</v>
+      </c>
+      <c r="V3" s="255" t="s">
         <v>493</v>
       </c>
-      <c r="V3" s="255" t="s">
+      <c r="W3" s="255" t="s">
         <v>494</v>
       </c>
-      <c r="W3" s="255" t="s">
+      <c r="X3" s="255" t="s">
         <v>49</v>
       </c>
-      <c r="X3" s="263" t="s">
+      <c r="Y3" s="263" t="s">
         <v>454</v>
       </c>
-      <c r="Y3" s="274" t="s">
+      <c r="Z3" s="274" t="s">
         <v>556</v>
       </c>
-      <c r="Z3" s="269" t="s">
+      <c r="AA3" s="269" t="s">
         <v>495</v>
       </c>
-      <c r="AA3" s="269" t="s">
+      <c r="AB3" s="269" t="s">
         <v>496</v>
       </c>
-      <c r="AB3" s="269" t="s">
+      <c r="AC3" s="269" t="s">
         <v>497</v>
       </c>
-      <c r="AC3" s="269" t="s">
+      <c r="AD3" s="269" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -18765,32 +18801,35 @@
         <v>550</v>
       </c>
       <c r="U4" s="256" t="s">
+        <v>587</v>
+      </c>
+      <c r="V4" s="256" t="s">
         <v>50</v>
       </c>
-      <c r="V4" s="256" t="s">
+      <c r="W4" s="256" t="s">
         <v>543</v>
       </c>
-      <c r="W4" s="256" t="s">
+      <c r="X4" s="256" t="s">
         <v>481</v>
       </c>
-      <c r="X4" s="260" t="s">
+      <c r="Y4" s="260" t="s">
         <v>23</v>
       </c>
-      <c r="Y4" s="276"/>
-      <c r="Z4" s="257" t="s">
+      <c r="Z4" s="276"/>
+      <c r="AA4" s="257" t="s">
         <v>408</v>
       </c>
-      <c r="AA4" s="264" t="s">
+      <c r="AB4" s="264" t="s">
         <v>503</v>
       </c>
-      <c r="AB4" s="268" t="s">
+      <c r="AC4" s="268" t="s">
         <v>499</v>
       </c>
-      <c r="AC4" s="267" t="s">
+      <c r="AD4" s="267" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -18839,32 +18878,35 @@
       </c>
       <c r="T5" s="273"/>
       <c r="U5" s="256" t="s">
+        <v>588</v>
+      </c>
+      <c r="V5" s="256" t="s">
         <v>380</v>
       </c>
-      <c r="V5" s="256" t="s">
+      <c r="W5" s="256" t="s">
         <v>489</v>
       </c>
-      <c r="W5" s="256" t="s">
+      <c r="X5" s="256" t="s">
         <v>546</v>
       </c>
-      <c r="X5" s="261" t="s">
+      <c r="Y5" s="261" t="s">
         <v>22</v>
       </c>
-      <c r="Y5" s="279"/>
-      <c r="Z5" s="257" t="s">
+      <c r="Z5" s="279"/>
+      <c r="AA5" s="257" t="s">
         <v>480</v>
       </c>
-      <c r="AA5" s="265" t="s">
+      <c r="AB5" s="265" t="s">
         <v>504</v>
       </c>
-      <c r="AB5" s="256" t="s">
+      <c r="AC5" s="256" t="s">
         <v>505</v>
       </c>
-      <c r="AC5" s="257" t="s">
+      <c r="AD5" s="257" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -18911,32 +18953,35 @@
         <v>552</v>
       </c>
       <c r="U6" s="256" t="s">
+        <v>589</v>
+      </c>
+      <c r="V6" s="256" t="s">
         <v>478</v>
       </c>
-      <c r="V6" s="256" t="s">
+      <c r="W6" s="256" t="s">
         <v>501</v>
       </c>
-      <c r="W6" s="256" t="s">
+      <c r="X6" s="256" t="s">
         <v>487</v>
       </c>
-      <c r="X6" s="261" t="s">
+      <c r="Y6" s="261" t="s">
         <v>23</v>
       </c>
-      <c r="Y6" s="281"/>
-      <c r="Z6" s="257" t="s">
+      <c r="Z6" s="281"/>
+      <c r="AA6" s="257" t="s">
         <v>413</v>
       </c>
-      <c r="AA6" s="265" t="s">
+      <c r="AB6" s="265" t="s">
         <v>507</v>
       </c>
-      <c r="AB6" s="256" t="s">
+      <c r="AC6" s="256" t="s">
         <v>508</v>
       </c>
-      <c r="AC6" s="257" t="s">
+      <c r="AD6" s="257" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
@@ -18985,32 +19030,35 @@
       </c>
       <c r="T7" s="273"/>
       <c r="U7" s="256" t="s">
+        <v>590</v>
+      </c>
+      <c r="V7" s="256" t="s">
         <v>473</v>
       </c>
-      <c r="V7" s="256" t="s">
+      <c r="W7" s="256" t="s">
         <v>491</v>
       </c>
-      <c r="W7" s="256" t="s">
+      <c r="X7" s="256" t="s">
         <v>547</v>
       </c>
-      <c r="X7" s="261" t="s">
+      <c r="Y7" s="261" t="s">
         <v>23</v>
       </c>
-      <c r="Y7" s="280"/>
-      <c r="Z7" s="257" t="s">
+      <c r="Z7" s="280"/>
+      <c r="AA7" s="257" t="s">
         <v>411</v>
       </c>
-      <c r="AA7" s="265" t="s">
+      <c r="AB7" s="265" t="s">
         <v>503</v>
       </c>
-      <c r="AB7" s="256" t="s">
+      <c r="AC7" s="256" t="s">
         <v>518</v>
       </c>
-      <c r="AC7" s="257" t="s">
+      <c r="AD7" s="257" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
@@ -19054,32 +19102,35 @@
         <v>554</v>
       </c>
       <c r="U8" s="256" t="s">
+        <v>591</v>
+      </c>
+      <c r="V8" s="256" t="s">
         <v>479</v>
       </c>
-      <c r="V8" s="256" t="s">
+      <c r="W8" s="256" t="s">
         <v>502</v>
       </c>
-      <c r="W8" s="256" t="s">
+      <c r="X8" s="256" t="s">
         <v>482</v>
       </c>
-      <c r="X8" s="261" t="s">
+      <c r="Y8" s="261" t="s">
         <v>16</v>
       </c>
-      <c r="Y8" s="277"/>
-      <c r="Z8" s="257" t="s">
+      <c r="Z8" s="277"/>
+      <c r="AA8" s="257" t="s">
         <v>548</v>
       </c>
-      <c r="AA8" s="265" t="s">
+      <c r="AB8" s="265" t="s">
         <v>503</v>
       </c>
-      <c r="AB8" s="256" t="s">
+      <c r="AC8" s="256" t="s">
         <v>522</v>
       </c>
-      <c r="AC8" s="257" t="s">
+      <c r="AD8" s="257" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>5</v>
       </c>
@@ -19122,33 +19173,36 @@
       <c r="T9" s="285" t="s">
         <v>558</v>
       </c>
-      <c r="U9" s="256" t="s">
+      <c r="U9" s="321" t="s">
+        <v>592</v>
+      </c>
+      <c r="V9" s="256" t="s">
         <v>377</v>
       </c>
-      <c r="V9" s="256" t="s">
+      <c r="W9" s="256" t="s">
         <v>490</v>
       </c>
-      <c r="W9" s="256" t="s">
+      <c r="X9" s="256" t="s">
         <v>483</v>
       </c>
-      <c r="X9" s="261" t="s">
+      <c r="Y9" s="261" t="s">
         <v>22</v>
       </c>
-      <c r="Y9" s="275"/>
-      <c r="Z9" s="257" t="s">
+      <c r="Z9" s="275"/>
+      <c r="AA9" s="257" t="s">
         <v>412</v>
       </c>
-      <c r="AA9" s="265" t="s">
+      <c r="AB9" s="265" t="s">
         <v>513</v>
       </c>
-      <c r="AB9" s="256" t="s">
+      <c r="AC9" s="256" t="s">
         <v>526</v>
       </c>
-      <c r="AC9" s="257" t="s">
+      <c r="AD9" s="257" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>7</v>
       </c>
@@ -19190,32 +19244,35 @@
       </c>
       <c r="T10" s="273"/>
       <c r="U10" s="256" t="s">
+        <v>593</v>
+      </c>
+      <c r="V10" s="256" t="s">
         <v>544</v>
       </c>
-      <c r="V10" s="256" t="s">
+      <c r="W10" s="256" t="s">
         <v>527</v>
       </c>
-      <c r="W10" s="256" t="s">
+      <c r="X10" s="256" t="s">
         <v>484</v>
       </c>
-      <c r="X10" s="261" t="s">
+      <c r="Y10" s="261" t="s">
         <v>22</v>
       </c>
-      <c r="Y10" s="283"/>
-      <c r="Z10" s="257" t="s">
+      <c r="Z10" s="283"/>
+      <c r="AA10" s="257" t="s">
         <v>414</v>
       </c>
-      <c r="AA10" s="265" t="s">
+      <c r="AB10" s="265" t="s">
         <v>515</v>
       </c>
-      <c r="AB10" s="256" t="s">
+      <c r="AC10" s="256" t="s">
         <v>516</v>
       </c>
-      <c r="AC10" s="257" t="s">
+      <c r="AD10" s="257" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>8</v>
       </c>
@@ -19250,32 +19307,35 @@
         <v>551</v>
       </c>
       <c r="U11" s="256" t="s">
+        <v>594</v>
+      </c>
+      <c r="V11" s="256" t="s">
         <v>378</v>
       </c>
-      <c r="V11" s="256" t="s">
+      <c r="W11" s="256" t="s">
         <v>492</v>
       </c>
-      <c r="W11" s="256" t="s">
+      <c r="X11" s="256" t="s">
         <v>485</v>
       </c>
-      <c r="X11" s="261" t="s">
+      <c r="Y11" s="261" t="s">
         <v>16</v>
       </c>
-      <c r="Y11" s="278"/>
-      <c r="Z11" s="257" t="s">
+      <c r="Z11" s="278"/>
+      <c r="AA11" s="257" t="s">
         <v>415</v>
       </c>
-      <c r="AA11" s="265" t="s">
+      <c r="AB11" s="265" t="s">
         <v>504</v>
       </c>
-      <c r="AB11" s="256" t="s">
+      <c r="AC11" s="256" t="s">
         <v>512</v>
       </c>
-      <c r="AC11" s="257" t="s">
+      <c r="AD11" s="257" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>9</v>
       </c>
@@ -19319,42 +19379,45 @@
         <v>555</v>
       </c>
       <c r="U12" s="258" t="s">
+        <v>595</v>
+      </c>
+      <c r="V12" s="258" t="s">
         <v>374</v>
       </c>
-      <c r="V12" s="258" t="s">
+      <c r="W12" s="258" t="s">
         <v>500</v>
       </c>
-      <c r="W12" s="258" t="s">
+      <c r="X12" s="258" t="s">
         <v>486</v>
       </c>
-      <c r="X12" s="262" t="s">
+      <c r="Y12" s="262" t="s">
         <v>16</v>
       </c>
-      <c r="Y12" s="282"/>
-      <c r="Z12" s="259" t="s">
+      <c r="Z12" s="282"/>
+      <c r="AA12" s="259" t="s">
         <v>416</v>
       </c>
-      <c r="AA12" s="266" t="s">
+      <c r="AB12" s="266" t="s">
         <v>503</v>
       </c>
-      <c r="AB12" s="258" t="s">
+      <c r="AC12" s="258" t="s">
         <v>519</v>
       </c>
-      <c r="AC12" s="259" t="s">
+      <c r="AD12" s="259" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="L14" s="234" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="L15" s="251" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="L16" s="254" t="s">
         <v>476</v>
       </c>
@@ -19363,9 +19426,9 @@
   <mergeCells count="6">
     <mergeCell ref="J2:N2"/>
     <mergeCell ref="A1:N1"/>
-    <mergeCell ref="R1:AC1"/>
-    <mergeCell ref="Z2:AC2"/>
-    <mergeCell ref="S2:Y2"/>
+    <mergeCell ref="R1:AD1"/>
+    <mergeCell ref="AA2:AD2"/>
+    <mergeCell ref="S2:Z2"/>
     <mergeCell ref="R2:R3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19392,23 +19455,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="290" t="s">
+      <c r="A1" s="292" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="290"/>
-      <c r="C1" s="290"/>
-      <c r="D1" s="290"/>
-      <c r="L1" s="290" t="s">
+      <c r="B1" s="292"/>
+      <c r="C1" s="292"/>
+      <c r="D1" s="292"/>
+      <c r="L1" s="292" t="s">
         <v>88</v>
       </c>
-      <c r="M1" s="290"/>
-      <c r="N1" s="290"/>
-      <c r="P1" s="290" t="s">
+      <c r="M1" s="292"/>
+      <c r="N1" s="292"/>
+      <c r="P1" s="292" t="s">
         <v>92</v>
       </c>
-      <c r="Q1" s="290"/>
-      <c r="R1" s="290"/>
-      <c r="S1" s="290"/>
+      <c r="Q1" s="292"/>
+      <c r="R1" s="292"/>
+      <c r="S1" s="292"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -19612,12 +19675,12 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="290" t="s">
+      <c r="A10" s="292" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="290"/>
-      <c r="C10" s="290"/>
-      <c r="D10" s="290"/>
+      <c r="B10" s="292"/>
+      <c r="C10" s="292"/>
+      <c r="D10" s="292"/>
       <c r="P10" t="s">
         <v>123</v>
       </c>
@@ -19993,14 +20056,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="302" t="s">
+      <c r="A1" s="304" t="s">
         <v>296</v>
       </c>
-      <c r="B1" s="302"/>
-      <c r="C1" s="302"/>
-      <c r="D1" s="302"/>
-      <c r="E1" s="302"/>
-      <c r="F1" s="302"/>
+      <c r="B1" s="304"/>
+      <c r="C1" s="304"/>
+      <c r="D1" s="304"/>
+      <c r="E1" s="304"/>
+      <c r="F1" s="304"/>
       <c r="G1" s="67"/>
       <c r="H1" s="67"/>
       <c r="I1" s="67"/>
@@ -21402,7 +21465,7 @@
       <c r="E76" s="223" t="s">
         <v>321</v>
       </c>
-      <c r="F76" s="303" t="s">
+      <c r="F76" s="305" t="s">
         <v>538</v>
       </c>
     </row>
@@ -21422,7 +21485,7 @@
       <c r="E77" s="223" t="s">
         <v>321</v>
       </c>
-      <c r="F77" s="304"/>
+      <c r="F77" s="306"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="236">
@@ -21440,7 +21503,7 @@
       <c r="E78" s="224" t="s">
         <v>322</v>
       </c>
-      <c r="F78" s="304"/>
+      <c r="F78" s="306"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="236">
@@ -21458,7 +21521,7 @@
       <c r="E79" s="224" t="s">
         <v>322</v>
       </c>
-      <c r="F79" s="305"/>
+      <c r="F79" s="307"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="237"/>
@@ -21596,14 +21659,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="302" t="s">
+      <c r="A1" s="304" t="s">
         <v>296</v>
       </c>
-      <c r="B1" s="302"/>
-      <c r="C1" s="302"/>
-      <c r="D1" s="302"/>
-      <c r="E1" s="302"/>
-      <c r="F1" s="302"/>
+      <c r="B1" s="304"/>
+      <c r="C1" s="304"/>
+      <c r="D1" s="304"/>
+      <c r="E1" s="304"/>
+      <c r="F1" s="304"/>
       <c r="G1" s="67"/>
       <c r="H1" s="67"/>
       <c r="I1" s="67"/>
@@ -23100,22 +23163,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="309" t="s">
+      <c r="A1" s="311" t="s">
         <v>296</v>
       </c>
-      <c r="B1" s="309"/>
-      <c r="C1" s="309"/>
-      <c r="D1" s="309"/>
-      <c r="E1" s="309"/>
-      <c r="F1" s="309"/>
-      <c r="G1" s="310"/>
-      <c r="H1" s="311" t="s">
+      <c r="B1" s="311"/>
+      <c r="C1" s="311"/>
+      <c r="D1" s="311"/>
+      <c r="E1" s="311"/>
+      <c r="F1" s="311"/>
+      <c r="G1" s="312"/>
+      <c r="H1" s="313" t="s">
         <v>328</v>
       </c>
-      <c r="I1" s="293"/>
-      <c r="J1" s="293"/>
-      <c r="K1" s="293"/>
-      <c r="L1" s="312"/>
+      <c r="I1" s="295"/>
+      <c r="J1" s="295"/>
+      <c r="K1" s="295"/>
+      <c r="L1" s="314"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="162" t="s">
@@ -23171,7 +23234,7 @@
       <c r="E3" s="73" t="s">
         <v>318</v>
       </c>
-      <c r="F3" s="306">
+      <c r="F3" s="308">
         <v>60</v>
       </c>
       <c r="G3" s="68">
@@ -23209,7 +23272,7 @@
       <c r="E4" s="74" t="s">
         <v>318</v>
       </c>
-      <c r="F4" s="307"/>
+      <c r="F4" s="310"/>
       <c r="G4" s="69">
         <v>30</v>
       </c>
@@ -23245,7 +23308,7 @@
       <c r="E5" s="74" t="s">
         <v>318</v>
       </c>
-      <c r="F5" s="307"/>
+      <c r="F5" s="310"/>
       <c r="G5" s="69">
         <v>20</v>
       </c>
@@ -23281,7 +23344,7 @@
       <c r="E6" s="74" t="s">
         <v>319</v>
       </c>
-      <c r="F6" s="307"/>
+      <c r="F6" s="310"/>
       <c r="G6" s="69">
         <v>10</v>
       </c>
@@ -23317,7 +23380,7 @@
       <c r="E7" s="74" t="s">
         <v>320</v>
       </c>
-      <c r="F7" s="308"/>
+      <c r="F7" s="309"/>
       <c r="G7" s="69">
         <v>5</v>
       </c>
@@ -23353,7 +23416,7 @@
       <c r="E8" s="75" t="s">
         <v>320</v>
       </c>
-      <c r="F8" s="306">
+      <c r="F8" s="308">
         <v>40</v>
       </c>
       <c r="G8" s="68">
@@ -23391,7 +23454,7 @@
       <c r="E9" s="76" t="s">
         <v>320</v>
       </c>
-      <c r="F9" s="307"/>
+      <c r="F9" s="310"/>
       <c r="G9" s="69">
         <v>40</v>
       </c>
@@ -23427,7 +23490,7 @@
       <c r="E10" s="77" t="s">
         <v>321</v>
       </c>
-      <c r="F10" s="308"/>
+      <c r="F10" s="309"/>
       <c r="G10" s="70">
         <v>20</v>
       </c>
@@ -23477,7 +23540,7 @@
       <c r="E12" s="78" t="s">
         <v>318</v>
       </c>
-      <c r="F12" s="306">
+      <c r="F12" s="308">
         <v>60</v>
       </c>
       <c r="G12" s="68">
@@ -23515,7 +23578,7 @@
       <c r="E13" s="79" t="s">
         <v>318</v>
       </c>
-      <c r="F13" s="307"/>
+      <c r="F13" s="310"/>
       <c r="G13" s="69">
         <v>20</v>
       </c>
@@ -23551,7 +23614,7 @@
       <c r="E14" s="79" t="s">
         <v>318</v>
       </c>
-      <c r="F14" s="307"/>
+      <c r="F14" s="310"/>
       <c r="G14" s="69">
         <v>25</v>
       </c>
@@ -23587,7 +23650,7 @@
       <c r="E15" s="79" t="s">
         <v>319</v>
       </c>
-      <c r="F15" s="307"/>
+      <c r="F15" s="310"/>
       <c r="G15" s="69">
         <v>15</v>
       </c>
@@ -23623,7 +23686,7 @@
       <c r="E16" s="79" t="s">
         <v>319</v>
       </c>
-      <c r="F16" s="307"/>
+      <c r="F16" s="310"/>
       <c r="G16" s="69">
         <v>10</v>
       </c>
@@ -23659,7 +23722,7 @@
       <c r="E17" s="79" t="s">
         <v>320</v>
       </c>
-      <c r="F17" s="308"/>
+      <c r="F17" s="309"/>
       <c r="G17" s="69">
         <v>5</v>
       </c>
@@ -23695,7 +23758,7 @@
       <c r="E18" s="80" t="s">
         <v>320</v>
       </c>
-      <c r="F18" s="306">
+      <c r="F18" s="308">
         <v>40</v>
       </c>
       <c r="G18" s="68">
@@ -23733,7 +23796,7 @@
       <c r="E19" s="81" t="s">
         <v>321</v>
       </c>
-      <c r="F19" s="307"/>
+      <c r="F19" s="310"/>
       <c r="G19" s="69">
         <v>20</v>
       </c>
@@ -23769,7 +23832,7 @@
       <c r="E20" s="82" t="s">
         <v>321</v>
       </c>
-      <c r="F20" s="308"/>
+      <c r="F20" s="309"/>
       <c r="G20" s="70">
         <v>10</v>
       </c>
@@ -23819,7 +23882,7 @@
       <c r="E22" s="83" t="s">
         <v>318</v>
       </c>
-      <c r="F22" s="306">
+      <c r="F22" s="308">
         <v>60</v>
       </c>
       <c r="G22" s="68">
@@ -23857,7 +23920,7 @@
       <c r="E23" s="84" t="s">
         <v>318</v>
       </c>
-      <c r="F23" s="307"/>
+      <c r="F23" s="310"/>
       <c r="G23" s="69">
         <v>60</v>
       </c>
@@ -23893,7 +23956,7 @@
       <c r="E24" s="84" t="s">
         <v>318</v>
       </c>
-      <c r="F24" s="307"/>
+      <c r="F24" s="310"/>
       <c r="G24" s="69">
         <v>15</v>
       </c>
@@ -23929,7 +23992,7 @@
       <c r="E25" s="84" t="s">
         <v>318</v>
       </c>
-      <c r="F25" s="307"/>
+      <c r="F25" s="310"/>
       <c r="G25" s="69">
         <v>5</v>
       </c>
@@ -23965,7 +24028,7 @@
       <c r="E26" s="110" t="s">
         <v>319</v>
       </c>
-      <c r="F26" s="306">
+      <c r="F26" s="308">
         <v>40</v>
       </c>
       <c r="G26" s="68">
@@ -24003,7 +24066,7 @@
       <c r="E27" s="85" t="s">
         <v>320</v>
       </c>
-      <c r="F27" s="307"/>
+      <c r="F27" s="310"/>
       <c r="G27" s="69">
         <v>50</v>
       </c>
@@ -24039,7 +24102,7 @@
       <c r="E28" s="86" t="s">
         <v>320</v>
       </c>
-      <c r="F28" s="308"/>
+      <c r="F28" s="309"/>
       <c r="G28" s="70">
         <v>20</v>
       </c>
@@ -24089,7 +24152,7 @@
       <c r="E30" s="87" t="s">
         <v>319</v>
       </c>
-      <c r="F30" s="306">
+      <c r="F30" s="308">
         <v>60</v>
       </c>
       <c r="G30" s="68">
@@ -24127,7 +24190,7 @@
       <c r="E31" s="88" t="s">
         <v>319</v>
       </c>
-      <c r="F31" s="307"/>
+      <c r="F31" s="310"/>
       <c r="G31" s="69">
         <v>60</v>
       </c>
@@ -24163,7 +24226,7 @@
       <c r="E32" s="88" t="s">
         <v>319</v>
       </c>
-      <c r="F32" s="307"/>
+      <c r="F32" s="310"/>
       <c r="G32" s="69">
         <v>15</v>
       </c>
@@ -24199,7 +24262,7 @@
       <c r="E33" s="88" t="s">
         <v>320</v>
       </c>
-      <c r="F33" s="307"/>
+      <c r="F33" s="310"/>
       <c r="G33" s="69">
         <v>10</v>
       </c>
@@ -24235,7 +24298,7 @@
       <c r="E34" s="88" t="s">
         <v>320</v>
       </c>
-      <c r="F34" s="307"/>
+      <c r="F34" s="310"/>
       <c r="G34" s="69">
         <v>5</v>
       </c>
@@ -24271,7 +24334,7 @@
       <c r="E35" s="114" t="s">
         <v>320</v>
       </c>
-      <c r="F35" s="306">
+      <c r="F35" s="308">
         <v>40</v>
       </c>
       <c r="G35" s="68">
@@ -24309,7 +24372,7 @@
       <c r="E36" s="89" t="s">
         <v>320</v>
       </c>
-      <c r="F36" s="307"/>
+      <c r="F36" s="310"/>
       <c r="G36" s="69">
         <v>70</v>
       </c>
@@ -24345,7 +24408,7 @@
       <c r="E37" s="90" t="s">
         <v>321</v>
       </c>
-      <c r="F37" s="308"/>
+      <c r="F37" s="309"/>
       <c r="G37" s="70">
         <v>10</v>
       </c>
@@ -24395,7 +24458,7 @@
       <c r="E39" s="91" t="s">
         <v>318</v>
       </c>
-      <c r="F39" s="306">
+      <c r="F39" s="308">
         <v>60</v>
       </c>
       <c r="G39" s="68">
@@ -24433,7 +24496,7 @@
       <c r="E40" s="92" t="s">
         <v>318</v>
       </c>
-      <c r="F40" s="307"/>
+      <c r="F40" s="310"/>
       <c r="G40" s="69">
         <v>50</v>
       </c>
@@ -24469,7 +24532,7 @@
       <c r="E41" s="92" t="s">
         <v>318</v>
       </c>
-      <c r="F41" s="307"/>
+      <c r="F41" s="310"/>
       <c r="G41" s="69">
         <v>20</v>
       </c>
@@ -24505,7 +24568,7 @@
       <c r="E42" s="92" t="s">
         <v>319</v>
       </c>
-      <c r="F42" s="307"/>
+      <c r="F42" s="310"/>
       <c r="G42" s="69">
         <v>10</v>
       </c>
@@ -24541,7 +24604,7 @@
       <c r="E43" s="118" t="s">
         <v>319</v>
       </c>
-      <c r="F43" s="306">
+      <c r="F43" s="308">
         <v>40</v>
       </c>
       <c r="G43" s="68">
@@ -24579,7 +24642,7 @@
       <c r="E44" s="93" t="s">
         <v>319</v>
       </c>
-      <c r="F44" s="307"/>
+      <c r="F44" s="310"/>
       <c r="G44" s="69">
         <v>10</v>
       </c>
@@ -24615,7 +24678,7 @@
       <c r="E45" s="93" t="s">
         <v>320</v>
       </c>
-      <c r="F45" s="307"/>
+      <c r="F45" s="310"/>
       <c r="G45" s="69">
         <v>30</v>
       </c>
@@ -24651,7 +24714,7 @@
       <c r="E46" s="94" t="s">
         <v>321</v>
       </c>
-      <c r="F46" s="308"/>
+      <c r="F46" s="309"/>
       <c r="G46" s="70">
         <v>10</v>
       </c>
@@ -24701,7 +24764,7 @@
       <c r="E48" s="95" t="s">
         <v>318</v>
       </c>
-      <c r="F48" s="306">
+      <c r="F48" s="308">
         <v>60</v>
       </c>
       <c r="G48" s="68">
@@ -24739,7 +24802,7 @@
       <c r="E49" s="96" t="s">
         <v>319</v>
       </c>
-      <c r="F49" s="307"/>
+      <c r="F49" s="310"/>
       <c r="G49" s="69">
         <v>20</v>
       </c>
@@ -24775,7 +24838,7 @@
       <c r="E50" s="96" t="s">
         <v>319</v>
       </c>
-      <c r="F50" s="307"/>
+      <c r="F50" s="310"/>
       <c r="G50" s="69">
         <v>10</v>
       </c>
@@ -24863,7 +24926,7 @@
       <c r="E53" s="97" t="s">
         <v>318</v>
       </c>
-      <c r="F53" s="306">
+      <c r="F53" s="308">
         <v>60</v>
       </c>
       <c r="G53" s="68">
@@ -24901,7 +24964,7 @@
       <c r="E54" s="98" t="s">
         <v>318</v>
       </c>
-      <c r="F54" s="307"/>
+      <c r="F54" s="310"/>
       <c r="G54" s="69">
         <v>20</v>
       </c>
@@ -24937,7 +25000,7 @@
       <c r="E55" s="98" t="s">
         <v>319</v>
       </c>
-      <c r="F55" s="307"/>
+      <c r="F55" s="310"/>
       <c r="G55" s="69">
         <v>10</v>
       </c>
@@ -24973,7 +25036,7 @@
       <c r="E56" s="125" t="s">
         <v>320</v>
       </c>
-      <c r="F56" s="306">
+      <c r="F56" s="308">
         <v>40</v>
       </c>
       <c r="G56" s="68">
@@ -25011,7 +25074,7 @@
       <c r="E57" s="99" t="s">
         <v>320</v>
       </c>
-      <c r="F57" s="307"/>
+      <c r="F57" s="310"/>
       <c r="G57" s="69">
         <v>15</v>
       </c>
@@ -25047,7 +25110,7 @@
       <c r="E58" s="100" t="s">
         <v>320</v>
       </c>
-      <c r="F58" s="308"/>
+      <c r="F58" s="309"/>
       <c r="G58" s="70">
         <v>5</v>
       </c>
@@ -25097,7 +25160,7 @@
       <c r="E60" s="101" t="s">
         <v>320</v>
       </c>
-      <c r="F60" s="306">
+      <c r="F60" s="308">
         <v>60</v>
       </c>
       <c r="G60" s="68">
@@ -25135,7 +25198,7 @@
       <c r="E61" s="102" t="s">
         <v>320</v>
       </c>
-      <c r="F61" s="307"/>
+      <c r="F61" s="310"/>
       <c r="G61" s="69">
         <v>20</v>
       </c>
@@ -25171,7 +25234,7 @@
       <c r="E62" s="102" t="s">
         <v>320</v>
       </c>
-      <c r="F62" s="307"/>
+      <c r="F62" s="310"/>
       <c r="G62" s="69">
         <v>20</v>
       </c>
@@ -25207,7 +25270,7 @@
       <c r="E63" s="102" t="s">
         <v>321</v>
       </c>
-      <c r="F63" s="307"/>
+      <c r="F63" s="310"/>
       <c r="G63" s="69">
         <v>15</v>
       </c>
@@ -25243,7 +25306,7 @@
       <c r="E64" s="102" t="s">
         <v>321</v>
       </c>
-      <c r="F64" s="307"/>
+      <c r="F64" s="310"/>
       <c r="G64" s="69">
         <v>15</v>
       </c>
@@ -25279,7 +25342,7 @@
       <c r="E65" s="102" t="s">
         <v>321</v>
       </c>
-      <c r="F65" s="307"/>
+      <c r="F65" s="310"/>
       <c r="G65" s="69">
         <v>10</v>
       </c>
@@ -25315,7 +25378,7 @@
       <c r="E66" s="128" t="s">
         <v>322</v>
       </c>
-      <c r="F66" s="306">
+      <c r="F66" s="308">
         <v>40</v>
       </c>
       <c r="G66" s="68">
@@ -25353,7 +25416,7 @@
       <c r="E67" s="103" t="s">
         <v>322</v>
       </c>
-      <c r="F67" s="308"/>
+      <c r="F67" s="309"/>
       <c r="G67" s="70">
         <v>20</v>
       </c>
@@ -25403,7 +25466,7 @@
       <c r="E69" s="104" t="s">
         <v>319</v>
       </c>
-      <c r="F69" s="306">
+      <c r="F69" s="308">
         <v>60</v>
       </c>
       <c r="G69" s="68">
@@ -25441,7 +25504,7 @@
       <c r="E70" s="105" t="s">
         <v>319</v>
       </c>
-      <c r="F70" s="307"/>
+      <c r="F70" s="310"/>
       <c r="G70" s="69">
         <v>35</v>
       </c>
@@ -25477,7 +25540,7 @@
       <c r="E71" s="105" t="s">
         <v>319</v>
       </c>
-      <c r="F71" s="307"/>
+      <c r="F71" s="310"/>
       <c r="G71" s="69">
         <v>20</v>
       </c>
@@ -25513,7 +25576,7 @@
       <c r="E72" s="105" t="s">
         <v>320</v>
       </c>
-      <c r="F72" s="307"/>
+      <c r="F72" s="310"/>
       <c r="G72" s="69">
         <v>10</v>
       </c>
@@ -25549,7 +25612,7 @@
       <c r="E73" s="130" t="s">
         <v>321</v>
       </c>
-      <c r="F73" s="306">
+      <c r="F73" s="308">
         <v>40</v>
       </c>
       <c r="G73" s="68">
@@ -25587,7 +25650,7 @@
       <c r="E74" s="106" t="s">
         <v>321</v>
       </c>
-      <c r="F74" s="308"/>
+      <c r="F74" s="309"/>
       <c r="G74" s="70">
         <v>75</v>
       </c>
@@ -25637,7 +25700,7 @@
       <c r="E76" s="107" t="s">
         <v>321</v>
       </c>
-      <c r="F76" s="307">
+      <c r="F76" s="310">
         <v>60</v>
       </c>
       <c r="G76" s="69">
@@ -25675,7 +25738,7 @@
       <c r="E77" s="107" t="s">
         <v>321</v>
       </c>
-      <c r="F77" s="307"/>
+      <c r="F77" s="310"/>
       <c r="G77" s="69">
         <v>75</v>
       </c>
@@ -25711,7 +25774,7 @@
       <c r="E78" s="132" t="s">
         <v>322</v>
       </c>
-      <c r="F78" s="306">
+      <c r="F78" s="308">
         <v>40</v>
       </c>
       <c r="G78" s="68">
@@ -25749,7 +25812,7 @@
       <c r="E79" s="108" t="s">
         <v>322</v>
       </c>
-      <c r="F79" s="308"/>
+      <c r="F79" s="309"/>
       <c r="G79" s="70">
         <v>75</v>
       </c>
@@ -25884,15 +25947,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="F73:F74"/>
-    <mergeCell ref="F76:F77"/>
-    <mergeCell ref="F78:F79"/>
-    <mergeCell ref="F48:F50"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="F56:F58"/>
-    <mergeCell ref="F60:F65"/>
-    <mergeCell ref="F66:F67"/>
-    <mergeCell ref="F69:F72"/>
     <mergeCell ref="F43:F46"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="H1:L1"/>
@@ -25905,6 +25959,15 @@
     <mergeCell ref="F30:F34"/>
     <mergeCell ref="F35:F37"/>
     <mergeCell ref="F39:F42"/>
+    <mergeCell ref="F73:F74"/>
+    <mergeCell ref="F76:F77"/>
+    <mergeCell ref="F78:F79"/>
+    <mergeCell ref="F48:F50"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="F56:F58"/>
+    <mergeCell ref="F60:F65"/>
+    <mergeCell ref="F66:F67"/>
+    <mergeCell ref="F69:F72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -25936,22 +25999,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="313" t="s">
+      <c r="A1" s="315" t="s">
         <v>296</v>
       </c>
-      <c r="B1" s="313"/>
-      <c r="C1" s="313"/>
-      <c r="D1" s="313"/>
-      <c r="E1" s="313"/>
-      <c r="F1" s="313"/>
-      <c r="G1" s="314"/>
-      <c r="H1" s="315" t="s">
+      <c r="B1" s="315"/>
+      <c r="C1" s="315"/>
+      <c r="D1" s="315"/>
+      <c r="E1" s="315"/>
+      <c r="F1" s="315"/>
+      <c r="G1" s="316"/>
+      <c r="H1" s="317" t="s">
         <v>328</v>
       </c>
-      <c r="I1" s="316"/>
-      <c r="J1" s="316"/>
-      <c r="K1" s="316"/>
-      <c r="L1" s="317"/>
+      <c r="I1" s="318"/>
+      <c r="J1" s="318"/>
+      <c r="K1" s="318"/>
+      <c r="L1" s="319"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="182" t="s">

</xml_diff>

<commit_message>
End of Day Commit; Entropy Grind Tmrw
</commit_message>
<xml_diff>
--- a/3. Scribbling/SamsaraExcel.xlsx
+++ b/3. Scribbling/SamsaraExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Drive\Writing Grand Compile\Repository\Project Samsara\Obsidian\ProjectSamsara\3. Scribbling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19251E3-FD3A-4A31-96CF-7AAFA9AD9292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9126233-E679-468B-8882-9715326B99C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="300" windowWidth="23256" windowHeight="12804" tabRatio="790" firstSheet="2" activeTab="2" xr2:uid="{E6D84C89-D0D8-4C46-AF33-8B126112E9FD}"/>
+    <workbookView xWindow="-108" yWindow="300" windowWidth="23256" windowHeight="12804" tabRatio="790" xr2:uid="{E6D84C89-D0D8-4C46-AF33-8B126112E9FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Workshop" sheetId="13" r:id="rId1"/>
@@ -1306,7 +1306,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2111" uniqueCount="648">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2178" uniqueCount="704">
   <si>
     <t>Tier</t>
   </si>
@@ -3266,6 +3266,174 @@
   </si>
   <si>
     <t>Lightning</t>
+  </si>
+  <si>
+    <t>5'0" - 5"5"</t>
+  </si>
+  <si>
+    <t>5'6" - 5'11"</t>
+  </si>
+  <si>
+    <t>6'0" - 6'5"</t>
+  </si>
+  <si>
+    <t>6'6" - 6'11"</t>
+  </si>
+  <si>
+    <t>7'0" - &gt;</t>
+  </si>
+  <si>
+    <t>4'6" - 4'11"</t>
+  </si>
+  <si>
+    <t>&gt; - 4'5"</t>
+  </si>
+  <si>
+    <t>51 - 75</t>
+  </si>
+  <si>
+    <t>76 - 100</t>
+  </si>
+  <si>
+    <t>101 - 125</t>
+  </si>
+  <si>
+    <t>126 - 150</t>
+  </si>
+  <si>
+    <t>151 - 175</t>
+  </si>
+  <si>
+    <t>176 - 200</t>
+  </si>
+  <si>
+    <t>201 - 225</t>
+  </si>
+  <si>
+    <t>226 - 250</t>
+  </si>
+  <si>
+    <t>Weight (kg)</t>
+  </si>
+  <si>
+    <t>&gt; - 50</t>
+  </si>
+  <si>
+    <t>251 - &gt;</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>Class T1</t>
+  </si>
+  <si>
+    <t>Class T2</t>
+  </si>
+  <si>
+    <t>Height (ft, in)</t>
+  </si>
+  <si>
+    <t>Class Contract.</t>
+  </si>
+  <si>
+    <t>Tall 3</t>
+  </si>
+  <si>
+    <t>Tall 2</t>
+  </si>
+  <si>
+    <t>Tall 1</t>
+  </si>
+  <si>
+    <t>Short 3</t>
+  </si>
+  <si>
+    <t>Short 2</t>
+  </si>
+  <si>
+    <t>Short 1</t>
+  </si>
+  <si>
+    <t>Average 0</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>Take Box B</t>
+  </si>
+  <si>
+    <t>Take Both</t>
+  </si>
+  <si>
+    <t>Predict B</t>
+  </si>
+  <si>
+    <t>Predict Both</t>
+  </si>
+  <si>
+    <t>A milly</t>
+  </si>
+  <si>
+    <t>Impossible</t>
+  </si>
+  <si>
+    <t>A thousand</t>
   </si>
 </sst>
 </file>
@@ -4356,16 +4524,56 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4394,6 +4602,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="35" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4446,49 +4657,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13336,10 +13504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF7F0CD0-2F4A-4BEA-A85E-51022C7A6842}">
-  <dimension ref="A2:D20"/>
+  <dimension ref="A2:D47"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13520,6 +13688,302 @@
       </c>
       <c r="D20" t="s">
         <v>582</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>685</v>
+      </c>
+      <c r="C22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>654</v>
+      </c>
+      <c r="C23" t="s">
+        <v>690</v>
+      </c>
+      <c r="D23" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>653</v>
+      </c>
+      <c r="C24" t="s">
+        <v>691</v>
+      </c>
+      <c r="D24" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>648</v>
+      </c>
+      <c r="C25" t="s">
+        <v>692</v>
+      </c>
+      <c r="D25" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26" t="s">
+        <v>649</v>
+      </c>
+      <c r="C26" t="s">
+        <v>693</v>
+      </c>
+      <c r="D26" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>650</v>
+      </c>
+      <c r="C27" t="s">
+        <v>689</v>
+      </c>
+      <c r="D27" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>6</v>
+      </c>
+      <c r="B28" t="s">
+        <v>651</v>
+      </c>
+      <c r="C28" t="s">
+        <v>688</v>
+      </c>
+      <c r="D28" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>7</v>
+      </c>
+      <c r="B29" t="s">
+        <v>652</v>
+      </c>
+      <c r="C29" t="s">
+        <v>687</v>
+      </c>
+      <c r="D29" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s">
+        <v>663</v>
+      </c>
+      <c r="C31" t="s">
+        <v>683</v>
+      </c>
+      <c r="D31" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" s="296" t="s">
+        <v>664</v>
+      </c>
+      <c r="C32" t="s">
+        <v>666</v>
+      </c>
+      <c r="D32" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33" s="296" t="s">
+        <v>655</v>
+      </c>
+      <c r="C33" t="s">
+        <v>668</v>
+      </c>
+      <c r="D33" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34" s="296" t="s">
+        <v>656</v>
+      </c>
+      <c r="C34" t="s">
+        <v>669</v>
+      </c>
+      <c r="D34" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35" s="296" t="s">
+        <v>657</v>
+      </c>
+      <c r="C35" t="s">
+        <v>670</v>
+      </c>
+      <c r="D35" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36" s="296" t="s">
+        <v>658</v>
+      </c>
+      <c r="C36" t="s">
+        <v>671</v>
+      </c>
+      <c r="D36" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>6</v>
+      </c>
+      <c r="B37" s="296" t="s">
+        <v>659</v>
+      </c>
+      <c r="C37" t="s">
+        <v>672</v>
+      </c>
+      <c r="D37" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>7</v>
+      </c>
+      <c r="B38" s="296" t="s">
+        <v>660</v>
+      </c>
+      <c r="C38" t="s">
+        <v>673</v>
+      </c>
+      <c r="D38" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>8</v>
+      </c>
+      <c r="B39" s="296" t="s">
+        <v>661</v>
+      </c>
+      <c r="C39" t="s">
+        <v>674</v>
+      </c>
+      <c r="D39" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>9</v>
+      </c>
+      <c r="B40" s="296" t="s">
+        <v>662</v>
+      </c>
+      <c r="C40" t="s">
+        <v>675</v>
+      </c>
+      <c r="D40" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>10</v>
+      </c>
+      <c r="B41" s="296" t="s">
+        <v>665</v>
+      </c>
+      <c r="C41" t="s">
+        <v>676</v>
+      </c>
+      <c r="D41" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>699</v>
+      </c>
+      <c r="D45" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>697</v>
+      </c>
+      <c r="C46" t="s">
+        <v>701</v>
+      </c>
+      <c r="D46" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>698</v>
+      </c>
+      <c r="C47" t="s">
+        <v>702</v>
+      </c>
+      <c r="D47" t="s">
+        <v>703</v>
       </c>
     </row>
   </sheetData>
@@ -13541,10 +14005,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A1" s="317" t="s">
+      <c r="A1" s="332" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="317"/>
+      <c r="B1" s="332"/>
       <c r="F1" t="s">
         <v>252</v>
       </c>
@@ -18204,10 +18668,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="317" t="s">
+      <c r="A1" s="332" t="s">
         <v>612</v>
       </c>
-      <c r="B1" s="317"/>
+      <c r="B1" s="332"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -18248,16 +18712,16 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="317" t="s">
+      <c r="A7" s="332" t="s">
         <v>613</v>
       </c>
-      <c r="B7" s="317"/>
+      <c r="B7" s="332"/>
     </row>
     <row r="8" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>608</v>
       </c>
-      <c r="B8" s="330" t="s">
+      <c r="B8" s="293" t="s">
         <v>611</v>
       </c>
     </row>
@@ -18265,7 +18729,7 @@
       <c r="A9" t="s">
         <v>609</v>
       </c>
-      <c r="B9" s="330" t="s">
+      <c r="B9" s="293" t="s">
         <v>639</v>
       </c>
     </row>
@@ -18273,15 +18737,15 @@
       <c r="A10" t="s">
         <v>610</v>
       </c>
-      <c r="B10" s="330" t="s">
+      <c r="B10" s="293" t="s">
         <v>639</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="317" t="s">
+      <c r="A12" s="332" t="s">
         <v>614</v>
       </c>
-      <c r="B12" s="317"/>
+      <c r="B12" s="332"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -18353,10 +18817,10 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="317" t="s">
+      <c r="A24" s="332" t="s">
         <v>632</v>
       </c>
-      <c r="B24" s="317"/>
+      <c r="B24" s="332"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -18443,149 +18907,149 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A1" s="288" t="s">
+      <c r="A1" s="297" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="290"/>
-      <c r="C1" s="290"/>
-      <c r="D1" s="291"/>
-      <c r="F1" s="318" t="s">
+      <c r="B1" s="298"/>
+      <c r="C1" s="298"/>
+      <c r="D1" s="299"/>
+      <c r="F1" s="303" t="s">
         <v>595</v>
       </c>
-      <c r="G1" s="319"/>
-      <c r="H1" s="319"/>
-      <c r="I1" s="319"/>
-      <c r="J1" s="319"/>
-      <c r="K1" s="319"/>
-      <c r="L1" s="329"/>
-      <c r="N1" s="318" t="s">
+      <c r="G1" s="304"/>
+      <c r="H1" s="304"/>
+      <c r="I1" s="304"/>
+      <c r="J1" s="304"/>
+      <c r="K1" s="304"/>
+      <c r="L1" s="305"/>
+      <c r="N1" s="303" t="s">
         <v>596</v>
       </c>
-      <c r="O1" s="319"/>
-      <c r="P1" s="319"/>
-      <c r="Q1" s="319"/>
-      <c r="R1" s="319"/>
-      <c r="S1" s="319"/>
-      <c r="T1" s="329"/>
-      <c r="V1" s="318" t="s">
+      <c r="O1" s="304"/>
+      <c r="P1" s="304"/>
+      <c r="Q1" s="304"/>
+      <c r="R1" s="304"/>
+      <c r="S1" s="304"/>
+      <c r="T1" s="305"/>
+      <c r="V1" s="303" t="s">
         <v>597</v>
       </c>
-      <c r="W1" s="319"/>
-      <c r="X1" s="319"/>
-      <c r="Y1" s="319"/>
-      <c r="Z1" s="319"/>
-      <c r="AA1" s="319"/>
-      <c r="AB1" s="329"/>
-      <c r="AD1" s="321" t="s">
+      <c r="W1" s="304"/>
+      <c r="X1" s="304"/>
+      <c r="Y1" s="304"/>
+      <c r="Z1" s="304"/>
+      <c r="AA1" s="304"/>
+      <c r="AB1" s="305"/>
+      <c r="AD1" s="300" t="s">
         <v>37</v>
       </c>
-      <c r="AE1" s="326"/>
-      <c r="AF1" s="326"/>
-      <c r="AG1" s="326"/>
-      <c r="AH1" s="326"/>
-      <c r="AI1" s="326"/>
-      <c r="AJ1" s="327"/>
+      <c r="AE1" s="301"/>
+      <c r="AF1" s="301"/>
+      <c r="AG1" s="301"/>
+      <c r="AH1" s="301"/>
+      <c r="AI1" s="301"/>
+      <c r="AJ1" s="302"/>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A2" s="328" t="s">
+      <c r="A2" s="292" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="328" t="s">
+      <c r="B2" s="292" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="328" t="s">
+      <c r="C2" s="292" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="328" t="s">
+      <c r="D2" s="292" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="328" t="s">
+      <c r="F2" s="292" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="328" t="s">
+      <c r="G2" s="292" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="328" t="s">
+      <c r="H2" s="292" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="328" t="s">
+      <c r="I2" s="292" t="s">
         <v>134</v>
       </c>
-      <c r="J2" s="328" t="s">
+      <c r="J2" s="292" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="328" t="s">
+      <c r="K2" s="292" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="328" t="s">
+      <c r="L2" s="292" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="328" t="s">
+      <c r="N2" s="292" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="328" t="s">
+      <c r="O2" s="292" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="328" t="s">
+      <c r="P2" s="292" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="328" t="s">
+      <c r="Q2" s="292" t="s">
         <v>134</v>
       </c>
-      <c r="R2" s="328" t="s">
+      <c r="R2" s="292" t="s">
         <v>33</v>
       </c>
-      <c r="S2" s="328" t="s">
+      <c r="S2" s="292" t="s">
         <v>0</v>
       </c>
-      <c r="T2" s="328" t="s">
+      <c r="T2" s="292" t="s">
         <v>3</v>
       </c>
-      <c r="V2" s="328" t="s">
+      <c r="V2" s="292" t="s">
         <v>8</v>
       </c>
-      <c r="W2" s="328" t="s">
+      <c r="W2" s="292" t="s">
         <v>9</v>
       </c>
-      <c r="X2" s="328" t="s">
+      <c r="X2" s="292" t="s">
         <v>2</v>
       </c>
-      <c r="Y2" s="328" t="s">
+      <c r="Y2" s="292" t="s">
         <v>134</v>
       </c>
-      <c r="Z2" s="328" t="s">
+      <c r="Z2" s="292" t="s">
         <v>33</v>
       </c>
-      <c r="AA2" s="328" t="s">
+      <c r="AA2" s="292" t="s">
         <v>0</v>
       </c>
-      <c r="AB2" s="328" t="s">
+      <c r="AB2" s="292" t="s">
         <v>3</v>
       </c>
-      <c r="AD2" s="322" t="s">
+      <c r="AD2" s="288" t="s">
         <v>8</v>
       </c>
-      <c r="AE2" s="322" t="s">
+      <c r="AE2" s="288" t="s">
         <v>9</v>
       </c>
-      <c r="AF2" s="322" t="s">
+      <c r="AF2" s="288" t="s">
         <v>2</v>
       </c>
-      <c r="AG2" s="322" t="s">
+      <c r="AG2" s="288" t="s">
         <v>43</v>
       </c>
-      <c r="AH2" s="322" t="s">
+      <c r="AH2" s="288" t="s">
         <v>0</v>
       </c>
-      <c r="AI2" s="322" t="s">
+      <c r="AI2" s="288" t="s">
         <v>45</v>
       </c>
-      <c r="AJ2" s="322" t="s">
+      <c r="AJ2" s="288" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A3" s="323">
+      <c r="A3" s="289">
         <v>1</v>
       </c>
       <c r="B3" s="6">
@@ -18597,7 +19061,7 @@
       <c r="D3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="324">
+      <c r="F3" s="290">
         <v>1</v>
       </c>
       <c r="G3" s="5" t="s">
@@ -18611,7 +19075,7 @@
         <v>1</v>
       </c>
       <c r="L3" s="10"/>
-      <c r="N3" s="324">
+      <c r="N3" s="290">
         <v>1</v>
       </c>
       <c r="O3" s="5" t="s">
@@ -18625,7 +19089,7 @@
         <v>1</v>
       </c>
       <c r="T3" s="10"/>
-      <c r="V3" s="324">
+      <c r="V3" s="290">
         <v>1</v>
       </c>
       <c r="W3" s="5" t="s">
@@ -18639,7 +19103,7 @@
         <v>1</v>
       </c>
       <c r="AB3" s="10"/>
-      <c r="AD3" s="324">
+      <c r="AD3" s="290">
         <v>23</v>
       </c>
       <c r="AE3" s="5" t="s">
@@ -18654,14 +19118,14 @@
       <c r="AJ3" s="10"/>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A4" s="323">
+      <c r="A4" s="289">
         <v>2</v>
       </c>
       <c r="B4" s="6">
         <v>25</v>
       </c>
       <c r="D4" s="8"/>
-      <c r="F4" s="323">
+      <c r="F4" s="289">
         <v>2</v>
       </c>
       <c r="G4" s="6" t="s">
@@ -18674,7 +19138,7 @@
         <v>1</v>
       </c>
       <c r="L4" s="8"/>
-      <c r="N4" s="323">
+      <c r="N4" s="289">
         <v>2</v>
       </c>
       <c r="O4" s="6" t="s">
@@ -18687,7 +19151,7 @@
         <v>1</v>
       </c>
       <c r="T4" s="8"/>
-      <c r="V4" s="323">
+      <c r="V4" s="289">
         <v>2</v>
       </c>
       <c r="W4" s="6" t="s">
@@ -18700,7 +19164,7 @@
         <v>1</v>
       </c>
       <c r="AB4" s="8"/>
-      <c r="AD4" s="323">
+      <c r="AD4" s="289">
         <v>24</v>
       </c>
       <c r="AE4" s="6" t="s">
@@ -18712,14 +19176,14 @@
       <c r="AJ4" s="8"/>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A5" s="323">
+      <c r="A5" s="289">
         <v>3</v>
       </c>
       <c r="B5" s="6">
         <v>12.5</v>
       </c>
       <c r="D5" s="8"/>
-      <c r="F5" s="323">
+      <c r="F5" s="289">
         <v>3</v>
       </c>
       <c r="G5" s="6" t="s">
@@ -18740,7 +19204,7 @@
       <c r="L5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="323">
+      <c r="N5" s="289">
         <v>3</v>
       </c>
       <c r="O5" s="6" t="s">
@@ -18753,7 +19217,7 @@
         <v>1</v>
       </c>
       <c r="T5" s="8"/>
-      <c r="V5" s="323">
+      <c r="V5" s="289">
         <v>3</v>
       </c>
       <c r="W5" s="6" t="s">
@@ -18766,7 +19230,7 @@
         <v>1</v>
       </c>
       <c r="AB5" s="8"/>
-      <c r="AD5" s="323">
+      <c r="AD5" s="289">
         <v>25</v>
       </c>
       <c r="AE5" s="6" t="s">
@@ -18778,14 +19242,14 @@
       <c r="AJ5" s="8"/>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A6" s="323">
+      <c r="A6" s="289">
         <v>4</v>
       </c>
       <c r="B6" s="6">
         <v>6.25</v>
       </c>
       <c r="D6" s="8"/>
-      <c r="F6" s="323">
+      <c r="F6" s="289">
         <v>4</v>
       </c>
       <c r="G6" s="6" t="s">
@@ -18798,7 +19262,7 @@
         <v>1</v>
       </c>
       <c r="L6" s="8"/>
-      <c r="N6" s="323">
+      <c r="N6" s="289">
         <v>4</v>
       </c>
       <c r="O6" s="6" t="s">
@@ -18811,7 +19275,7 @@
         <v>1</v>
       </c>
       <c r="T6" s="8"/>
-      <c r="V6" s="323">
+      <c r="V6" s="289">
         <v>4</v>
       </c>
       <c r="W6" s="6" t="s">
@@ -18824,7 +19288,7 @@
         <v>1</v>
       </c>
       <c r="AB6" s="8"/>
-      <c r="AD6" s="325">
+      <c r="AD6" s="291">
         <v>26</v>
       </c>
       <c r="AE6" s="7" t="s">
@@ -18847,14 +19311,14 @@
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A7" s="323">
+      <c r="A7" s="289">
         <v>5</v>
       </c>
       <c r="B7" s="6">
         <v>3.125</v>
       </c>
       <c r="D7" s="8"/>
-      <c r="F7" s="323">
+      <c r="F7" s="289">
         <v>5</v>
       </c>
       <c r="G7" s="6" t="s">
@@ -18867,7 +19331,7 @@
         <v>1</v>
       </c>
       <c r="L7" s="8"/>
-      <c r="N7" s="323">
+      <c r="N7" s="289">
         <v>5</v>
       </c>
       <c r="O7" s="6" t="s">
@@ -18880,7 +19344,7 @@
         <v>1</v>
       </c>
       <c r="T7" s="8"/>
-      <c r="V7" s="323">
+      <c r="V7" s="289">
         <v>5</v>
       </c>
       <c r="W7" s="6" t="s">
@@ -18895,14 +19359,14 @@
       <c r="AB7" s="8"/>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A8" s="323">
+      <c r="A8" s="289">
         <v>6</v>
       </c>
       <c r="B8" s="6">
         <v>1.5625</v>
       </c>
       <c r="D8" s="8"/>
-      <c r="F8" s="323">
+      <c r="F8" s="289">
         <v>6</v>
       </c>
       <c r="G8" s="6" t="s">
@@ -18915,7 +19379,7 @@
         <v>1</v>
       </c>
       <c r="L8" s="8"/>
-      <c r="N8" s="323">
+      <c r="N8" s="289">
         <v>6</v>
       </c>
       <c r="O8" s="6" t="s">
@@ -18928,7 +19392,7 @@
         <v>1</v>
       </c>
       <c r="T8" s="8"/>
-      <c r="V8" s="323">
+      <c r="V8" s="289">
         <v>6</v>
       </c>
       <c r="W8" s="6" t="s">
@@ -18943,14 +19407,14 @@
       <c r="AB8" s="8"/>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A9" s="323">
+      <c r="A9" s="289">
         <v>7</v>
       </c>
       <c r="B9" s="6">
         <v>0.78125</v>
       </c>
       <c r="D9" s="8"/>
-      <c r="F9" s="323">
+      <c r="F9" s="289">
         <v>7</v>
       </c>
       <c r="G9" s="6" t="s">
@@ -18963,7 +19427,7 @@
         <v>2</v>
       </c>
       <c r="L9" s="8"/>
-      <c r="N9" s="323">
+      <c r="N9" s="289">
         <v>7</v>
       </c>
       <c r="O9" s="6" t="s">
@@ -18976,7 +19440,7 @@
         <v>2</v>
       </c>
       <c r="T9" s="8"/>
-      <c r="V9" s="323">
+      <c r="V9" s="289">
         <v>7</v>
       </c>
       <c r="W9" s="6" t="s">
@@ -18991,7 +19455,7 @@
       <c r="AB9" s="8"/>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A10" s="325">
+      <c r="A10" s="291">
         <v>8</v>
       </c>
       <c r="B10" s="7">
@@ -19003,7 +19467,7 @@
       <c r="D10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="323">
+      <c r="F10" s="289">
         <v>8</v>
       </c>
       <c r="G10" s="6" t="s">
@@ -19016,7 +19480,7 @@
         <v>2</v>
       </c>
       <c r="L10" s="8"/>
-      <c r="N10" s="323">
+      <c r="N10" s="289">
         <v>8</v>
       </c>
       <c r="O10" s="6" t="s">
@@ -19029,7 +19493,7 @@
         <v>2</v>
       </c>
       <c r="T10" s="8"/>
-      <c r="V10" s="323">
+      <c r="V10" s="289">
         <v>8</v>
       </c>
       <c r="W10" s="6" t="s">
@@ -19044,7 +19508,7 @@
       <c r="AB10" s="8"/>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="F11" s="323">
+      <c r="F11" s="289">
         <v>9</v>
       </c>
       <c r="G11" s="6" t="s">
@@ -19057,7 +19521,7 @@
         <v>2</v>
       </c>
       <c r="L11" s="8"/>
-      <c r="N11" s="323">
+      <c r="N11" s="289">
         <v>9</v>
       </c>
       <c r="O11" s="6" t="s">
@@ -19070,7 +19534,7 @@
         <v>2</v>
       </c>
       <c r="T11" s="8"/>
-      <c r="V11" s="323">
+      <c r="V11" s="289">
         <v>9</v>
       </c>
       <c r="W11" s="6" t="s">
@@ -19085,7 +19549,7 @@
       <c r="AB11" s="8"/>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="F12" s="323">
+      <c r="F12" s="289">
         <v>10</v>
       </c>
       <c r="G12" s="6" t="s">
@@ -19098,7 +19562,7 @@
         <v>2</v>
       </c>
       <c r="L12" s="8"/>
-      <c r="N12" s="323">
+      <c r="N12" s="289">
         <v>10</v>
       </c>
       <c r="O12" s="6" t="s">
@@ -19111,7 +19575,7 @@
         <v>2</v>
       </c>
       <c r="T12" s="8"/>
-      <c r="V12" s="323">
+      <c r="V12" s="289">
         <v>10</v>
       </c>
       <c r="W12" s="6" t="s">
@@ -19126,7 +19590,7 @@
       <c r="AB12" s="8"/>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="F13" s="323">
+      <c r="F13" s="289">
         <v>11</v>
       </c>
       <c r="G13" s="6" t="s">
@@ -19139,7 +19603,7 @@
         <v>3</v>
       </c>
       <c r="L13" s="8"/>
-      <c r="N13" s="323">
+      <c r="N13" s="289">
         <v>11</v>
       </c>
       <c r="O13" s="6" t="s">
@@ -19152,7 +19616,7 @@
         <v>3</v>
       </c>
       <c r="T13" s="8"/>
-      <c r="V13" s="323">
+      <c r="V13" s="289">
         <v>11</v>
       </c>
       <c r="W13" s="6" t="s">
@@ -19167,7 +19631,7 @@
       <c r="AB13" s="8"/>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="F14" s="325">
+      <c r="F14" s="291">
         <v>12</v>
       </c>
       <c r="G14" s="7" t="s">
@@ -19182,7 +19646,7 @@
         <v>3</v>
       </c>
       <c r="L14" s="9"/>
-      <c r="N14" s="325">
+      <c r="N14" s="291">
         <v>12</v>
       </c>
       <c r="O14" s="7" t="s">
@@ -19197,7 +19661,7 @@
         <v>3</v>
       </c>
       <c r="T14" s="9"/>
-      <c r="V14" s="325">
+      <c r="V14" s="291">
         <v>12</v>
       </c>
       <c r="W14" s="7" t="s">
@@ -19219,7 +19683,7 @@
       <c r="Y15" s="7"/>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="F16" s="324">
+      <c r="F16" s="290">
         <v>13</v>
       </c>
       <c r="G16" s="5" t="s">
@@ -19233,7 +19697,7 @@
         <v>1</v>
       </c>
       <c r="L16" s="10"/>
-      <c r="N16" s="324">
+      <c r="N16" s="290">
         <v>13</v>
       </c>
       <c r="O16" s="5" t="s">
@@ -19247,7 +19711,7 @@
         <v>1</v>
       </c>
       <c r="T16" s="10"/>
-      <c r="V16" s="324">
+      <c r="V16" s="290">
         <v>13</v>
       </c>
       <c r="W16" s="5" t="s">
@@ -19263,7 +19727,7 @@
       <c r="AB16" s="10"/>
     </row>
     <row r="17" spans="6:28" x14ac:dyDescent="0.3">
-      <c r="F17" s="323">
+      <c r="F17" s="289">
         <v>14</v>
       </c>
       <c r="G17" s="6" t="s">
@@ -19276,26 +19740,26 @@
         <v>1</v>
       </c>
       <c r="L17" s="8"/>
-      <c r="N17" s="323">
+      <c r="N17" s="289">
         <v>14</v>
       </c>
       <c r="O17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="R17" s="320" t="s">
+      <c r="R17" s="6" t="s">
         <v>34</v>
       </c>
       <c r="S17" s="6">
         <v>1</v>
       </c>
       <c r="T17" s="8"/>
-      <c r="V17" s="323">
+      <c r="V17" s="289">
         <v>14</v>
       </c>
       <c r="W17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Z17" s="320" t="s">
+      <c r="Z17" s="6" t="s">
         <v>36</v>
       </c>
       <c r="AA17" s="6">
@@ -19304,7 +19768,7 @@
       <c r="AB17" s="8"/>
     </row>
     <row r="18" spans="6:28" x14ac:dyDescent="0.3">
-      <c r="F18" s="323">
+      <c r="F18" s="289">
         <v>15</v>
       </c>
       <c r="G18" s="6" t="s">
@@ -19317,26 +19781,26 @@
         <v>1</v>
       </c>
       <c r="L18" s="8"/>
-      <c r="N18" s="323">
+      <c r="N18" s="289">
         <v>15</v>
       </c>
       <c r="O18" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="R18" s="320" t="s">
+      <c r="R18" s="6" t="s">
         <v>34</v>
       </c>
       <c r="S18" s="6">
         <v>1</v>
       </c>
       <c r="T18" s="8"/>
-      <c r="V18" s="323">
+      <c r="V18" s="289">
         <v>15</v>
       </c>
       <c r="W18" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="Z18" s="320" t="s">
+      <c r="Z18" s="6" t="s">
         <v>36</v>
       </c>
       <c r="AA18" s="6">
@@ -19345,7 +19809,7 @@
       <c r="AB18" s="8"/>
     </row>
     <row r="19" spans="6:28" x14ac:dyDescent="0.3">
-      <c r="F19" s="323">
+      <c r="F19" s="289">
         <v>16</v>
       </c>
       <c r="G19" s="6" t="s">
@@ -19358,26 +19822,26 @@
         <v>2</v>
       </c>
       <c r="L19" s="8"/>
-      <c r="N19" s="323">
+      <c r="N19" s="289">
         <v>16</v>
       </c>
       <c r="O19" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="R19" s="320" t="s">
+      <c r="R19" s="6" t="s">
         <v>34</v>
       </c>
       <c r="S19" s="6">
         <v>2</v>
       </c>
       <c r="T19" s="8"/>
-      <c r="V19" s="323">
+      <c r="V19" s="289">
         <v>16</v>
       </c>
       <c r="W19" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="Z19" s="320" t="s">
+      <c r="Z19" s="6" t="s">
         <v>36</v>
       </c>
       <c r="AA19" s="6">
@@ -19386,7 +19850,7 @@
       <c r="AB19" s="8"/>
     </row>
     <row r="20" spans="6:28" x14ac:dyDescent="0.3">
-      <c r="F20" s="323">
+      <c r="F20" s="289">
         <v>17</v>
       </c>
       <c r="G20" s="6" t="s">
@@ -19399,26 +19863,26 @@
         <v>2</v>
       </c>
       <c r="L20" s="8"/>
-      <c r="N20" s="323">
+      <c r="N20" s="289">
         <v>17</v>
       </c>
       <c r="O20" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="R20" s="320" t="s">
+      <c r="R20" s="6" t="s">
         <v>34</v>
       </c>
       <c r="S20" s="6">
         <v>2</v>
       </c>
       <c r="T20" s="8"/>
-      <c r="V20" s="323">
+      <c r="V20" s="289">
         <v>17</v>
       </c>
       <c r="W20" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="Z20" s="320" t="s">
+      <c r="Z20" s="6" t="s">
         <v>36</v>
       </c>
       <c r="AA20" s="6">
@@ -19427,7 +19891,7 @@
       <c r="AB20" s="8"/>
     </row>
     <row r="21" spans="6:28" x14ac:dyDescent="0.3">
-      <c r="F21" s="325">
+      <c r="F21" s="291">
         <v>18</v>
       </c>
       <c r="G21" s="7" t="s">
@@ -19442,7 +19906,7 @@
         <v>3</v>
       </c>
       <c r="L21" s="9"/>
-      <c r="N21" s="325">
+      <c r="N21" s="291">
         <v>18</v>
       </c>
       <c r="O21" s="7" t="s">
@@ -19457,7 +19921,7 @@
         <v>3</v>
       </c>
       <c r="T21" s="9"/>
-      <c r="V21" s="325">
+      <c r="V21" s="291">
         <v>18</v>
       </c>
       <c r="W21" s="7" t="s">
@@ -19479,7 +19943,7 @@
       <c r="Y22" s="7"/>
     </row>
     <row r="23" spans="6:28" x14ac:dyDescent="0.3">
-      <c r="F23" s="324">
+      <c r="F23" s="290">
         <v>19</v>
       </c>
       <c r="G23" s="5" t="s">
@@ -19493,7 +19957,7 @@
         <v>1</v>
       </c>
       <c r="L23" s="10"/>
-      <c r="N23" s="324">
+      <c r="N23" s="290">
         <v>19</v>
       </c>
       <c r="O23" s="5" t="s">
@@ -19507,7 +19971,7 @@
         <v>1</v>
       </c>
       <c r="T23" s="10"/>
-      <c r="V23" s="324">
+      <c r="V23" s="290">
         <v>19</v>
       </c>
       <c r="W23" s="5" t="s">
@@ -19523,7 +19987,7 @@
       <c r="AB23" s="10"/>
     </row>
     <row r="24" spans="6:28" x14ac:dyDescent="0.3">
-      <c r="F24" s="323">
+      <c r="F24" s="289">
         <v>20</v>
       </c>
       <c r="G24" s="6" t="s">
@@ -19536,26 +20000,26 @@
         <v>1</v>
       </c>
       <c r="L24" s="8"/>
-      <c r="N24" s="323">
+      <c r="N24" s="289">
         <v>20</v>
       </c>
       <c r="O24" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="R24" s="320" t="s">
+      <c r="R24" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S24" s="6">
         <v>1</v>
       </c>
       <c r="T24" s="8"/>
-      <c r="V24" s="323">
+      <c r="V24" s="289">
         <v>20</v>
       </c>
       <c r="W24" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="Z24" s="320" t="s">
+      <c r="Z24" s="6" t="s">
         <v>34</v>
       </c>
       <c r="AA24" s="6">
@@ -19564,7 +20028,7 @@
       <c r="AB24" s="8"/>
     </row>
     <row r="25" spans="6:28" x14ac:dyDescent="0.3">
-      <c r="F25" s="323">
+      <c r="F25" s="289">
         <v>21</v>
       </c>
       <c r="G25" s="6" t="s">
@@ -19577,26 +20041,26 @@
         <v>2</v>
       </c>
       <c r="L25" s="8"/>
-      <c r="N25" s="323">
+      <c r="N25" s="289">
         <v>21</v>
       </c>
       <c r="O25" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="R25" s="320" t="s">
+      <c r="R25" s="6" t="s">
         <v>35</v>
       </c>
       <c r="S25" s="6">
         <v>2</v>
       </c>
       <c r="T25" s="8"/>
-      <c r="V25" s="323">
+      <c r="V25" s="289">
         <v>21</v>
       </c>
       <c r="W25" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="Z25" s="320" t="s">
+      <c r="Z25" s="6" t="s">
         <v>34</v>
       </c>
       <c r="AA25" s="6">
@@ -19605,7 +20069,7 @@
       <c r="AB25" s="8"/>
     </row>
     <row r="26" spans="6:28" x14ac:dyDescent="0.3">
-      <c r="F26" s="325">
+      <c r="F26" s="291">
         <v>22</v>
       </c>
       <c r="G26" s="7" t="s">
@@ -19620,7 +20084,7 @@
         <v>3</v>
       </c>
       <c r="L26" s="9"/>
-      <c r="N26" s="325">
+      <c r="N26" s="291">
         <v>22</v>
       </c>
       <c r="O26" s="7" t="s">
@@ -19635,7 +20099,7 @@
         <v>3</v>
       </c>
       <c r="T26" s="9"/>
-      <c r="V26" s="325">
+      <c r="V26" s="291">
         <v>22</v>
       </c>
       <c r="W26" s="7" t="s">
@@ -19679,7 +20143,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7594C28-F5C4-4873-B2AF-F5CC5CA2F682}">
   <dimension ref="A1:AD23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="104" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScale="104" workbookViewId="0">
       <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
@@ -19707,65 +20171,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="292" t="s">
+      <c r="A1" s="306" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="292"/>
-      <c r="C1" s="292"/>
-      <c r="D1" s="292"/>
-      <c r="E1" s="292"/>
-      <c r="F1" s="292"/>
-      <c r="G1" s="292"/>
-      <c r="H1" s="292"/>
-      <c r="I1" s="292"/>
-      <c r="J1" s="292"/>
-      <c r="K1" s="292"/>
-      <c r="L1" s="292"/>
-      <c r="M1" s="292"/>
-      <c r="N1" s="292"/>
-      <c r="R1" s="293" t="s">
+      <c r="B1" s="306"/>
+      <c r="C1" s="306"/>
+      <c r="D1" s="306"/>
+      <c r="E1" s="306"/>
+      <c r="F1" s="306"/>
+      <c r="G1" s="306"/>
+      <c r="H1" s="306"/>
+      <c r="I1" s="306"/>
+      <c r="J1" s="306"/>
+      <c r="K1" s="306"/>
+      <c r="L1" s="306"/>
+      <c r="M1" s="306"/>
+      <c r="N1" s="306"/>
+      <c r="R1" s="307" t="s">
         <v>487</v>
       </c>
-      <c r="S1" s="294"/>
-      <c r="T1" s="294"/>
-      <c r="U1" s="294"/>
-      <c r="V1" s="294"/>
-      <c r="W1" s="294"/>
-      <c r="X1" s="294"/>
-      <c r="Y1" s="294"/>
-      <c r="Z1" s="294"/>
-      <c r="AA1" s="294"/>
-      <c r="AB1" s="294"/>
-      <c r="AC1" s="294"/>
-      <c r="AD1" s="295"/>
+      <c r="S1" s="308"/>
+      <c r="T1" s="308"/>
+      <c r="U1" s="308"/>
+      <c r="V1" s="308"/>
+      <c r="W1" s="308"/>
+      <c r="X1" s="308"/>
+      <c r="Y1" s="308"/>
+      <c r="Z1" s="308"/>
+      <c r="AA1" s="308"/>
+      <c r="AB1" s="308"/>
+      <c r="AC1" s="308"/>
+      <c r="AD1" s="309"/>
     </row>
     <row r="2" spans="1:30" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J2" s="292" t="s">
+      <c r="J2" s="306" t="s">
         <v>422</v>
       </c>
-      <c r="K2" s="292"/>
-      <c r="L2" s="292"/>
-      <c r="M2" s="292"/>
-      <c r="N2" s="292"/>
-      <c r="R2" s="299" t="s">
+      <c r="K2" s="306"/>
+      <c r="L2" s="306"/>
+      <c r="M2" s="306"/>
+      <c r="N2" s="306"/>
+      <c r="R2" s="313" t="s">
         <v>8</v>
       </c>
-      <c r="S2" s="297" t="s">
+      <c r="S2" s="311" t="s">
         <v>524</v>
       </c>
-      <c r="T2" s="297"/>
-      <c r="U2" s="297"/>
-      <c r="V2" s="297"/>
-      <c r="W2" s="297"/>
-      <c r="X2" s="297"/>
-      <c r="Y2" s="297"/>
-      <c r="Z2" s="298"/>
-      <c r="AA2" s="296" t="s">
+      <c r="T2" s="311"/>
+      <c r="U2" s="311"/>
+      <c r="V2" s="311"/>
+      <c r="W2" s="311"/>
+      <c r="X2" s="311"/>
+      <c r="Y2" s="311"/>
+      <c r="Z2" s="312"/>
+      <c r="AA2" s="310" t="s">
         <v>523</v>
       </c>
-      <c r="AB2" s="297"/>
-      <c r="AC2" s="297"/>
-      <c r="AD2" s="298"/>
+      <c r="AB2" s="311"/>
+      <c r="AC2" s="311"/>
+      <c r="AD2" s="312"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -19804,7 +20268,7 @@
       <c r="N3" s="231">
         <v>5</v>
       </c>
-      <c r="R3" s="300"/>
+      <c r="R3" s="314"/>
       <c r="S3" s="282" t="s">
         <v>2</v>
       </c>
@@ -20500,7 +20964,7 @@
       <c r="L14" s="232" t="s">
         <v>473</v>
       </c>
-      <c r="R14" s="331" t="s">
+      <c r="R14" s="294" t="s">
         <v>8</v>
       </c>
       <c r="S14" s="282" t="s">
@@ -20512,7 +20976,7 @@
       <c r="U14" s="261" t="s">
         <v>453</v>
       </c>
-      <c r="V14" s="332" t="s">
+      <c r="V14" s="295" t="s">
         <v>640</v>
       </c>
     </row>
@@ -20532,7 +20996,7 @@
       <c r="U15" s="258" t="s">
         <v>22</v>
       </c>
-      <c r="V15" s="332" t="s">
+      <c r="V15" s="295" t="s">
         <v>641</v>
       </c>
     </row>
@@ -20552,7 +21016,7 @@
       <c r="U16" s="259" t="s">
         <v>21</v>
       </c>
-      <c r="V16" s="332" t="s">
+      <c r="V16" s="295" t="s">
         <v>642</v>
       </c>
     </row>
@@ -20583,7 +21047,7 @@
       <c r="U18" s="259" t="s">
         <v>22</v>
       </c>
-      <c r="V18" s="332" t="s">
+      <c r="V18" s="295" t="s">
         <v>646</v>
       </c>
     </row>
@@ -20600,7 +21064,7 @@
       <c r="U19" s="259" t="s">
         <v>15</v>
       </c>
-      <c r="V19" s="332" t="s">
+      <c r="V19" s="295" t="s">
         <v>644</v>
       </c>
     </row>
@@ -20634,7 +21098,7 @@
       <c r="U21" s="259" t="s">
         <v>21</v>
       </c>
-      <c r="V21" s="332" t="s">
+      <c r="V21" s="295" t="s">
         <v>647</v>
       </c>
     </row>
@@ -20702,23 +21166,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="289" t="s">
+      <c r="A1" s="315" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="289"/>
-      <c r="C1" s="289"/>
-      <c r="D1" s="289"/>
-      <c r="L1" s="289" t="s">
+      <c r="B1" s="315"/>
+      <c r="C1" s="315"/>
+      <c r="D1" s="315"/>
+      <c r="L1" s="315" t="s">
         <v>87</v>
       </c>
-      <c r="M1" s="289"/>
-      <c r="N1" s="289"/>
-      <c r="P1" s="289" t="s">
+      <c r="M1" s="315"/>
+      <c r="N1" s="315"/>
+      <c r="P1" s="315" t="s">
         <v>91</v>
       </c>
-      <c r="Q1" s="289"/>
-      <c r="R1" s="289"/>
-      <c r="S1" s="289"/>
+      <c r="Q1" s="315"/>
+      <c r="R1" s="315"/>
+      <c r="S1" s="315"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -20922,12 +21386,12 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="289" t="s">
+      <c r="A10" s="315" t="s">
         <v>82</v>
       </c>
-      <c r="B10" s="289"/>
-      <c r="C10" s="289"/>
-      <c r="D10" s="289"/>
+      <c r="B10" s="315"/>
+      <c r="C10" s="315"/>
+      <c r="D10" s="315"/>
       <c r="P10" t="s">
         <v>122</v>
       </c>
@@ -21303,14 +21767,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="301" t="s">
+      <c r="A1" s="316" t="s">
         <v>295</v>
       </c>
-      <c r="B1" s="301"/>
-      <c r="C1" s="301"/>
-      <c r="D1" s="301"/>
-      <c r="E1" s="301"/>
-      <c r="F1" s="301"/>
+      <c r="B1" s="316"/>
+      <c r="C1" s="316"/>
+      <c r="D1" s="316"/>
+      <c r="E1" s="316"/>
+      <c r="F1" s="316"/>
       <c r="G1" s="65"/>
       <c r="H1" s="65"/>
       <c r="I1" s="65"/>
@@ -22712,7 +23176,7 @@
       <c r="E76" s="221" t="s">
         <v>320</v>
       </c>
-      <c r="F76" s="302" t="s">
+      <c r="F76" s="317" t="s">
         <v>537</v>
       </c>
     </row>
@@ -22732,7 +23196,7 @@
       <c r="E77" s="221" t="s">
         <v>320</v>
       </c>
-      <c r="F77" s="303"/>
+      <c r="F77" s="318"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="234">
@@ -22750,7 +23214,7 @@
       <c r="E78" s="222" t="s">
         <v>321</v>
       </c>
-      <c r="F78" s="303"/>
+      <c r="F78" s="318"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="234">
@@ -22768,7 +23232,7 @@
       <c r="E79" s="222" t="s">
         <v>321</v>
       </c>
-      <c r="F79" s="304"/>
+      <c r="F79" s="319"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="235"/>
@@ -22906,14 +23370,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="301" t="s">
+      <c r="A1" s="316" t="s">
         <v>295</v>
       </c>
-      <c r="B1" s="301"/>
-      <c r="C1" s="301"/>
-      <c r="D1" s="301"/>
-      <c r="E1" s="301"/>
-      <c r="F1" s="301"/>
+      <c r="B1" s="316"/>
+      <c r="C1" s="316"/>
+      <c r="D1" s="316"/>
+      <c r="E1" s="316"/>
+      <c r="F1" s="316"/>
       <c r="G1" s="65"/>
       <c r="H1" s="65"/>
       <c r="I1" s="65"/>
@@ -24410,22 +24874,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="308" t="s">
+      <c r="A1" s="323" t="s">
         <v>295</v>
       </c>
-      <c r="B1" s="308"/>
-      <c r="C1" s="308"/>
-      <c r="D1" s="308"/>
-      <c r="E1" s="308"/>
-      <c r="F1" s="308"/>
-      <c r="G1" s="309"/>
-      <c r="H1" s="310" t="s">
+      <c r="B1" s="323"/>
+      <c r="C1" s="323"/>
+      <c r="D1" s="323"/>
+      <c r="E1" s="323"/>
+      <c r="F1" s="323"/>
+      <c r="G1" s="324"/>
+      <c r="H1" s="325" t="s">
         <v>327</v>
       </c>
-      <c r="I1" s="292"/>
-      <c r="J1" s="292"/>
-      <c r="K1" s="292"/>
-      <c r="L1" s="311"/>
+      <c r="I1" s="306"/>
+      <c r="J1" s="306"/>
+      <c r="K1" s="306"/>
+      <c r="L1" s="326"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="160" t="s">
@@ -24481,7 +24945,7 @@
       <c r="E3" s="71" t="s">
         <v>317</v>
       </c>
-      <c r="F3" s="305">
+      <c r="F3" s="320">
         <v>60</v>
       </c>
       <c r="G3" s="66">
@@ -24519,7 +24983,7 @@
       <c r="E4" s="72" t="s">
         <v>317</v>
       </c>
-      <c r="F4" s="306"/>
+      <c r="F4" s="321"/>
       <c r="G4" s="67">
         <v>30</v>
       </c>
@@ -24555,7 +25019,7 @@
       <c r="E5" s="72" t="s">
         <v>317</v>
       </c>
-      <c r="F5" s="306"/>
+      <c r="F5" s="321"/>
       <c r="G5" s="67">
         <v>20</v>
       </c>
@@ -24591,7 +25055,7 @@
       <c r="E6" s="72" t="s">
         <v>318</v>
       </c>
-      <c r="F6" s="306"/>
+      <c r="F6" s="321"/>
       <c r="G6" s="67">
         <v>10</v>
       </c>
@@ -24627,7 +25091,7 @@
       <c r="E7" s="72" t="s">
         <v>319</v>
       </c>
-      <c r="F7" s="307"/>
+      <c r="F7" s="322"/>
       <c r="G7" s="67">
         <v>5</v>
       </c>
@@ -24663,7 +25127,7 @@
       <c r="E8" s="73" t="s">
         <v>319</v>
       </c>
-      <c r="F8" s="305">
+      <c r="F8" s="320">
         <v>40</v>
       </c>
       <c r="G8" s="66">
@@ -24701,7 +25165,7 @@
       <c r="E9" s="74" t="s">
         <v>319</v>
       </c>
-      <c r="F9" s="306"/>
+      <c r="F9" s="321"/>
       <c r="G9" s="67">
         <v>40</v>
       </c>
@@ -24737,7 +25201,7 @@
       <c r="E10" s="75" t="s">
         <v>320</v>
       </c>
-      <c r="F10" s="307"/>
+      <c r="F10" s="322"/>
       <c r="G10" s="68">
         <v>20</v>
       </c>
@@ -24787,7 +25251,7 @@
       <c r="E12" s="76" t="s">
         <v>317</v>
       </c>
-      <c r="F12" s="305">
+      <c r="F12" s="320">
         <v>60</v>
       </c>
       <c r="G12" s="66">
@@ -24825,7 +25289,7 @@
       <c r="E13" s="77" t="s">
         <v>317</v>
       </c>
-      <c r="F13" s="306"/>
+      <c r="F13" s="321"/>
       <c r="G13" s="67">
         <v>20</v>
       </c>
@@ -24861,7 +25325,7 @@
       <c r="E14" s="77" t="s">
         <v>317</v>
       </c>
-      <c r="F14" s="306"/>
+      <c r="F14" s="321"/>
       <c r="G14" s="67">
         <v>25</v>
       </c>
@@ -24897,7 +25361,7 @@
       <c r="E15" s="77" t="s">
         <v>318</v>
       </c>
-      <c r="F15" s="306"/>
+      <c r="F15" s="321"/>
       <c r="G15" s="67">
         <v>15</v>
       </c>
@@ -24933,7 +25397,7 @@
       <c r="E16" s="77" t="s">
         <v>318</v>
       </c>
-      <c r="F16" s="306"/>
+      <c r="F16" s="321"/>
       <c r="G16" s="67">
         <v>10</v>
       </c>
@@ -24969,7 +25433,7 @@
       <c r="E17" s="77" t="s">
         <v>319</v>
       </c>
-      <c r="F17" s="307"/>
+      <c r="F17" s="322"/>
       <c r="G17" s="67">
         <v>5</v>
       </c>
@@ -25005,7 +25469,7 @@
       <c r="E18" s="78" t="s">
         <v>319</v>
       </c>
-      <c r="F18" s="305">
+      <c r="F18" s="320">
         <v>40</v>
       </c>
       <c r="G18" s="66">
@@ -25043,7 +25507,7 @@
       <c r="E19" s="79" t="s">
         <v>320</v>
       </c>
-      <c r="F19" s="306"/>
+      <c r="F19" s="321"/>
       <c r="G19" s="67">
         <v>20</v>
       </c>
@@ -25079,7 +25543,7 @@
       <c r="E20" s="80" t="s">
         <v>320</v>
       </c>
-      <c r="F20" s="307"/>
+      <c r="F20" s="322"/>
       <c r="G20" s="68">
         <v>10</v>
       </c>
@@ -25129,7 +25593,7 @@
       <c r="E22" s="81" t="s">
         <v>317</v>
       </c>
-      <c r="F22" s="305">
+      <c r="F22" s="320">
         <v>60</v>
       </c>
       <c r="G22" s="66">
@@ -25167,7 +25631,7 @@
       <c r="E23" s="82" t="s">
         <v>317</v>
       </c>
-      <c r="F23" s="306"/>
+      <c r="F23" s="321"/>
       <c r="G23" s="67">
         <v>60</v>
       </c>
@@ -25203,7 +25667,7 @@
       <c r="E24" s="82" t="s">
         <v>317</v>
       </c>
-      <c r="F24" s="306"/>
+      <c r="F24" s="321"/>
       <c r="G24" s="67">
         <v>15</v>
       </c>
@@ -25239,7 +25703,7 @@
       <c r="E25" s="82" t="s">
         <v>317</v>
       </c>
-      <c r="F25" s="306"/>
+      <c r="F25" s="321"/>
       <c r="G25" s="67">
         <v>5</v>
       </c>
@@ -25275,7 +25739,7 @@
       <c r="E26" s="108" t="s">
         <v>318</v>
       </c>
-      <c r="F26" s="305">
+      <c r="F26" s="320">
         <v>40</v>
       </c>
       <c r="G26" s="66">
@@ -25313,7 +25777,7 @@
       <c r="E27" s="83" t="s">
         <v>319</v>
       </c>
-      <c r="F27" s="306"/>
+      <c r="F27" s="321"/>
       <c r="G27" s="67">
         <v>50</v>
       </c>
@@ -25349,7 +25813,7 @@
       <c r="E28" s="84" t="s">
         <v>319</v>
       </c>
-      <c r="F28" s="307"/>
+      <c r="F28" s="322"/>
       <c r="G28" s="68">
         <v>20</v>
       </c>
@@ -25399,7 +25863,7 @@
       <c r="E30" s="85" t="s">
         <v>318</v>
       </c>
-      <c r="F30" s="305">
+      <c r="F30" s="320">
         <v>60</v>
       </c>
       <c r="G30" s="66">
@@ -25437,7 +25901,7 @@
       <c r="E31" s="86" t="s">
         <v>318</v>
       </c>
-      <c r="F31" s="306"/>
+      <c r="F31" s="321"/>
       <c r="G31" s="67">
         <v>60</v>
       </c>
@@ -25473,7 +25937,7 @@
       <c r="E32" s="86" t="s">
         <v>318</v>
       </c>
-      <c r="F32" s="306"/>
+      <c r="F32" s="321"/>
       <c r="G32" s="67">
         <v>15</v>
       </c>
@@ -25509,7 +25973,7 @@
       <c r="E33" s="86" t="s">
         <v>319</v>
       </c>
-      <c r="F33" s="306"/>
+      <c r="F33" s="321"/>
       <c r="G33" s="67">
         <v>10</v>
       </c>
@@ -25545,7 +26009,7 @@
       <c r="E34" s="86" t="s">
         <v>319</v>
       </c>
-      <c r="F34" s="306"/>
+      <c r="F34" s="321"/>
       <c r="G34" s="67">
         <v>5</v>
       </c>
@@ -25581,7 +26045,7 @@
       <c r="E35" s="112" t="s">
         <v>319</v>
       </c>
-      <c r="F35" s="305">
+      <c r="F35" s="320">
         <v>40</v>
       </c>
       <c r="G35" s="66">
@@ -25619,7 +26083,7 @@
       <c r="E36" s="87" t="s">
         <v>319</v>
       </c>
-      <c r="F36" s="306"/>
+      <c r="F36" s="321"/>
       <c r="G36" s="67">
         <v>70</v>
       </c>
@@ -25655,7 +26119,7 @@
       <c r="E37" s="88" t="s">
         <v>320</v>
       </c>
-      <c r="F37" s="307"/>
+      <c r="F37" s="322"/>
       <c r="G37" s="68">
         <v>10</v>
       </c>
@@ -25705,7 +26169,7 @@
       <c r="E39" s="89" t="s">
         <v>317</v>
       </c>
-      <c r="F39" s="305">
+      <c r="F39" s="320">
         <v>60</v>
       </c>
       <c r="G39" s="66">
@@ -25743,7 +26207,7 @@
       <c r="E40" s="90" t="s">
         <v>317</v>
       </c>
-      <c r="F40" s="306"/>
+      <c r="F40" s="321"/>
       <c r="G40" s="67">
         <v>50</v>
       </c>
@@ -25779,7 +26243,7 @@
       <c r="E41" s="90" t="s">
         <v>317</v>
       </c>
-      <c r="F41" s="306"/>
+      <c r="F41" s="321"/>
       <c r="G41" s="67">
         <v>20</v>
       </c>
@@ -25815,7 +26279,7 @@
       <c r="E42" s="90" t="s">
         <v>318</v>
       </c>
-      <c r="F42" s="306"/>
+      <c r="F42" s="321"/>
       <c r="G42" s="67">
         <v>10</v>
       </c>
@@ -25851,7 +26315,7 @@
       <c r="E43" s="116" t="s">
         <v>318</v>
       </c>
-      <c r="F43" s="305">
+      <c r="F43" s="320">
         <v>40</v>
       </c>
       <c r="G43" s="66">
@@ -25889,7 +26353,7 @@
       <c r="E44" s="91" t="s">
         <v>318</v>
       </c>
-      <c r="F44" s="306"/>
+      <c r="F44" s="321"/>
       <c r="G44" s="67">
         <v>10</v>
       </c>
@@ -25925,7 +26389,7 @@
       <c r="E45" s="91" t="s">
         <v>319</v>
       </c>
-      <c r="F45" s="306"/>
+      <c r="F45" s="321"/>
       <c r="G45" s="67">
         <v>30</v>
       </c>
@@ -25961,7 +26425,7 @@
       <c r="E46" s="92" t="s">
         <v>320</v>
       </c>
-      <c r="F46" s="307"/>
+      <c r="F46" s="322"/>
       <c r="G46" s="68">
         <v>10</v>
       </c>
@@ -26011,7 +26475,7 @@
       <c r="E48" s="93" t="s">
         <v>317</v>
       </c>
-      <c r="F48" s="305">
+      <c r="F48" s="320">
         <v>60</v>
       </c>
       <c r="G48" s="66">
@@ -26049,7 +26513,7 @@
       <c r="E49" s="94" t="s">
         <v>318</v>
       </c>
-      <c r="F49" s="306"/>
+      <c r="F49" s="321"/>
       <c r="G49" s="67">
         <v>20</v>
       </c>
@@ -26085,7 +26549,7 @@
       <c r="E50" s="94" t="s">
         <v>318</v>
       </c>
-      <c r="F50" s="306"/>
+      <c r="F50" s="321"/>
       <c r="G50" s="67">
         <v>10</v>
       </c>
@@ -26173,7 +26637,7 @@
       <c r="E53" s="95" t="s">
         <v>317</v>
       </c>
-      <c r="F53" s="305">
+      <c r="F53" s="320">
         <v>60</v>
       </c>
       <c r="G53" s="66">
@@ -26211,7 +26675,7 @@
       <c r="E54" s="96" t="s">
         <v>317</v>
       </c>
-      <c r="F54" s="306"/>
+      <c r="F54" s="321"/>
       <c r="G54" s="67">
         <v>20</v>
       </c>
@@ -26247,7 +26711,7 @@
       <c r="E55" s="96" t="s">
         <v>318</v>
       </c>
-      <c r="F55" s="306"/>
+      <c r="F55" s="321"/>
       <c r="G55" s="67">
         <v>10</v>
       </c>
@@ -26283,7 +26747,7 @@
       <c r="E56" s="123" t="s">
         <v>319</v>
       </c>
-      <c r="F56" s="305">
+      <c r="F56" s="320">
         <v>40</v>
       </c>
       <c r="G56" s="66">
@@ -26321,7 +26785,7 @@
       <c r="E57" s="97" t="s">
         <v>319</v>
       </c>
-      <c r="F57" s="306"/>
+      <c r="F57" s="321"/>
       <c r="G57" s="67">
         <v>15</v>
       </c>
@@ -26357,7 +26821,7 @@
       <c r="E58" s="98" t="s">
         <v>319</v>
       </c>
-      <c r="F58" s="307"/>
+      <c r="F58" s="322"/>
       <c r="G58" s="68">
         <v>5</v>
       </c>
@@ -26407,7 +26871,7 @@
       <c r="E60" s="99" t="s">
         <v>319</v>
       </c>
-      <c r="F60" s="305">
+      <c r="F60" s="320">
         <v>60</v>
       </c>
       <c r="G60" s="66">
@@ -26445,7 +26909,7 @@
       <c r="E61" s="100" t="s">
         <v>319</v>
       </c>
-      <c r="F61" s="306"/>
+      <c r="F61" s="321"/>
       <c r="G61" s="67">
         <v>20</v>
       </c>
@@ -26481,7 +26945,7 @@
       <c r="E62" s="100" t="s">
         <v>319</v>
       </c>
-      <c r="F62" s="306"/>
+      <c r="F62" s="321"/>
       <c r="G62" s="67">
         <v>20</v>
       </c>
@@ -26517,7 +26981,7 @@
       <c r="E63" s="100" t="s">
         <v>320</v>
       </c>
-      <c r="F63" s="306"/>
+      <c r="F63" s="321"/>
       <c r="G63" s="67">
         <v>15</v>
       </c>
@@ -26553,7 +27017,7 @@
       <c r="E64" s="100" t="s">
         <v>320</v>
       </c>
-      <c r="F64" s="306"/>
+      <c r="F64" s="321"/>
       <c r="G64" s="67">
         <v>15</v>
       </c>
@@ -26589,7 +27053,7 @@
       <c r="E65" s="100" t="s">
         <v>320</v>
       </c>
-      <c r="F65" s="306"/>
+      <c r="F65" s="321"/>
       <c r="G65" s="67">
         <v>10</v>
       </c>
@@ -26625,7 +27089,7 @@
       <c r="E66" s="126" t="s">
         <v>321</v>
       </c>
-      <c r="F66" s="305">
+      <c r="F66" s="320">
         <v>40</v>
       </c>
       <c r="G66" s="66">
@@ -26663,7 +27127,7 @@
       <c r="E67" s="101" t="s">
         <v>321</v>
       </c>
-      <c r="F67" s="307"/>
+      <c r="F67" s="322"/>
       <c r="G67" s="68">
         <v>20</v>
       </c>
@@ -26713,7 +27177,7 @@
       <c r="E69" s="102" t="s">
         <v>318</v>
       </c>
-      <c r="F69" s="305">
+      <c r="F69" s="320">
         <v>60</v>
       </c>
       <c r="G69" s="66">
@@ -26751,7 +27215,7 @@
       <c r="E70" s="103" t="s">
         <v>318</v>
       </c>
-      <c r="F70" s="306"/>
+      <c r="F70" s="321"/>
       <c r="G70" s="67">
         <v>35</v>
       </c>
@@ -26787,7 +27251,7 @@
       <c r="E71" s="103" t="s">
         <v>318</v>
       </c>
-      <c r="F71" s="306"/>
+      <c r="F71" s="321"/>
       <c r="G71" s="67">
         <v>20</v>
       </c>
@@ -26823,7 +27287,7 @@
       <c r="E72" s="103" t="s">
         <v>319</v>
       </c>
-      <c r="F72" s="306"/>
+      <c r="F72" s="321"/>
       <c r="G72" s="67">
         <v>10</v>
       </c>
@@ -26859,7 +27323,7 @@
       <c r="E73" s="128" t="s">
         <v>320</v>
       </c>
-      <c r="F73" s="305">
+      <c r="F73" s="320">
         <v>40</v>
       </c>
       <c r="G73" s="66">
@@ -26897,7 +27361,7 @@
       <c r="E74" s="104" t="s">
         <v>320</v>
       </c>
-      <c r="F74" s="307"/>
+      <c r="F74" s="322"/>
       <c r="G74" s="68">
         <v>75</v>
       </c>
@@ -26947,7 +27411,7 @@
       <c r="E76" s="105" t="s">
         <v>320</v>
       </c>
-      <c r="F76" s="306">
+      <c r="F76" s="321">
         <v>60</v>
       </c>
       <c r="G76" s="67">
@@ -26985,7 +27449,7 @@
       <c r="E77" s="105" t="s">
         <v>320</v>
       </c>
-      <c r="F77" s="306"/>
+      <c r="F77" s="321"/>
       <c r="G77" s="67">
         <v>75</v>
       </c>
@@ -27021,7 +27485,7 @@
       <c r="E78" s="130" t="s">
         <v>321</v>
       </c>
-      <c r="F78" s="305">
+      <c r="F78" s="320">
         <v>40</v>
       </c>
       <c r="G78" s="66">
@@ -27059,7 +27523,7 @@
       <c r="E79" s="106" t="s">
         <v>321</v>
       </c>
-      <c r="F79" s="307"/>
+      <c r="F79" s="322"/>
       <c r="G79" s="68">
         <v>75</v>
       </c>
@@ -27246,22 +27710,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="312" t="s">
+      <c r="A1" s="327" t="s">
         <v>295</v>
       </c>
-      <c r="B1" s="312"/>
-      <c r="C1" s="312"/>
-      <c r="D1" s="312"/>
-      <c r="E1" s="312"/>
-      <c r="F1" s="312"/>
-      <c r="G1" s="313"/>
-      <c r="H1" s="314" t="s">
+      <c r="B1" s="327"/>
+      <c r="C1" s="327"/>
+      <c r="D1" s="327"/>
+      <c r="E1" s="327"/>
+      <c r="F1" s="327"/>
+      <c r="G1" s="328"/>
+      <c r="H1" s="329" t="s">
         <v>327</v>
       </c>
-      <c r="I1" s="315"/>
-      <c r="J1" s="315"/>
-      <c r="K1" s="315"/>
-      <c r="L1" s="316"/>
+      <c r="I1" s="330"/>
+      <c r="J1" s="330"/>
+      <c r="K1" s="330"/>
+      <c r="L1" s="331"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="180" t="s">

</xml_diff>

<commit_message>
ACs, Void, Upping the WN-DT
</commit_message>
<xml_diff>
--- a/3. Scribbling/SamsaraExcel.xlsx
+++ b/3. Scribbling/SamsaraExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Drive\Writing Grand Compile\Repository\Project Samsara\Obsidian\ProjectSamsara\3. Scribbling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9126233-E679-468B-8882-9715326B99C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0130B884-5076-4342-9D56-0BB2DE9D8F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="300" windowWidth="23256" windowHeight="12804" tabRatio="790" xr2:uid="{E6D84C89-D0D8-4C46-AF33-8B126112E9FD}"/>
+    <workbookView xWindow="-108" yWindow="300" windowWidth="23256" windowHeight="12804" tabRatio="790" activeTab="2" xr2:uid="{E6D84C89-D0D8-4C46-AF33-8B126112E9FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Workshop" sheetId="13" r:id="rId1"/>
@@ -4621,10 +4621,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -13506,7 +13506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF7F0CD0-2F4A-4BEA-A85E-51022C7A6842}">
   <dimension ref="A2:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
@@ -20143,8 +20143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7594C28-F5C4-4873-B2AF-F5CC5CA2F682}">
   <dimension ref="A1:AD23"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="W18" sqref="W18"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="104" workbookViewId="0">
+      <selection activeCell="W17" sqref="W17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24983,7 +24983,7 @@
       <c r="E4" s="72" t="s">
         <v>317</v>
       </c>
-      <c r="F4" s="321"/>
+      <c r="F4" s="322"/>
       <c r="G4" s="67">
         <v>30</v>
       </c>
@@ -25019,7 +25019,7 @@
       <c r="E5" s="72" t="s">
         <v>317</v>
       </c>
-      <c r="F5" s="321"/>
+      <c r="F5" s="322"/>
       <c r="G5" s="67">
         <v>20</v>
       </c>
@@ -25055,7 +25055,7 @@
       <c r="E6" s="72" t="s">
         <v>318</v>
       </c>
-      <c r="F6" s="321"/>
+      <c r="F6" s="322"/>
       <c r="G6" s="67">
         <v>10</v>
       </c>
@@ -25091,7 +25091,7 @@
       <c r="E7" s="72" t="s">
         <v>319</v>
       </c>
-      <c r="F7" s="322"/>
+      <c r="F7" s="321"/>
       <c r="G7" s="67">
         <v>5</v>
       </c>
@@ -25165,7 +25165,7 @@
       <c r="E9" s="74" t="s">
         <v>319</v>
       </c>
-      <c r="F9" s="321"/>
+      <c r="F9" s="322"/>
       <c r="G9" s="67">
         <v>40</v>
       </c>
@@ -25201,7 +25201,7 @@
       <c r="E10" s="75" t="s">
         <v>320</v>
       </c>
-      <c r="F10" s="322"/>
+      <c r="F10" s="321"/>
       <c r="G10" s="68">
         <v>20</v>
       </c>
@@ -25289,7 +25289,7 @@
       <c r="E13" s="77" t="s">
         <v>317</v>
       </c>
-      <c r="F13" s="321"/>
+      <c r="F13" s="322"/>
       <c r="G13" s="67">
         <v>20</v>
       </c>
@@ -25325,7 +25325,7 @@
       <c r="E14" s="77" t="s">
         <v>317</v>
       </c>
-      <c r="F14" s="321"/>
+      <c r="F14" s="322"/>
       <c r="G14" s="67">
         <v>25</v>
       </c>
@@ -25361,7 +25361,7 @@
       <c r="E15" s="77" t="s">
         <v>318</v>
       </c>
-      <c r="F15" s="321"/>
+      <c r="F15" s="322"/>
       <c r="G15" s="67">
         <v>15</v>
       </c>
@@ -25397,7 +25397,7 @@
       <c r="E16" s="77" t="s">
         <v>318</v>
       </c>
-      <c r="F16" s="321"/>
+      <c r="F16" s="322"/>
       <c r="G16" s="67">
         <v>10</v>
       </c>
@@ -25433,7 +25433,7 @@
       <c r="E17" s="77" t="s">
         <v>319</v>
       </c>
-      <c r="F17" s="322"/>
+      <c r="F17" s="321"/>
       <c r="G17" s="67">
         <v>5</v>
       </c>
@@ -25507,7 +25507,7 @@
       <c r="E19" s="79" t="s">
         <v>320</v>
       </c>
-      <c r="F19" s="321"/>
+      <c r="F19" s="322"/>
       <c r="G19" s="67">
         <v>20</v>
       </c>
@@ -25543,7 +25543,7 @@
       <c r="E20" s="80" t="s">
         <v>320</v>
       </c>
-      <c r="F20" s="322"/>
+      <c r="F20" s="321"/>
       <c r="G20" s="68">
         <v>10</v>
       </c>
@@ -25631,7 +25631,7 @@
       <c r="E23" s="82" t="s">
         <v>317</v>
       </c>
-      <c r="F23" s="321"/>
+      <c r="F23" s="322"/>
       <c r="G23" s="67">
         <v>60</v>
       </c>
@@ -25667,7 +25667,7 @@
       <c r="E24" s="82" t="s">
         <v>317</v>
       </c>
-      <c r="F24" s="321"/>
+      <c r="F24" s="322"/>
       <c r="G24" s="67">
         <v>15</v>
       </c>
@@ -25703,7 +25703,7 @@
       <c r="E25" s="82" t="s">
         <v>317</v>
       </c>
-      <c r="F25" s="321"/>
+      <c r="F25" s="322"/>
       <c r="G25" s="67">
         <v>5</v>
       </c>
@@ -25777,7 +25777,7 @@
       <c r="E27" s="83" t="s">
         <v>319</v>
       </c>
-      <c r="F27" s="321"/>
+      <c r="F27" s="322"/>
       <c r="G27" s="67">
         <v>50</v>
       </c>
@@ -25813,7 +25813,7 @@
       <c r="E28" s="84" t="s">
         <v>319</v>
       </c>
-      <c r="F28" s="322"/>
+      <c r="F28" s="321"/>
       <c r="G28" s="68">
         <v>20</v>
       </c>
@@ -25901,7 +25901,7 @@
       <c r="E31" s="86" t="s">
         <v>318</v>
       </c>
-      <c r="F31" s="321"/>
+      <c r="F31" s="322"/>
       <c r="G31" s="67">
         <v>60</v>
       </c>
@@ -25937,7 +25937,7 @@
       <c r="E32" s="86" t="s">
         <v>318</v>
       </c>
-      <c r="F32" s="321"/>
+      <c r="F32" s="322"/>
       <c r="G32" s="67">
         <v>15</v>
       </c>
@@ -25973,7 +25973,7 @@
       <c r="E33" s="86" t="s">
         <v>319</v>
       </c>
-      <c r="F33" s="321"/>
+      <c r="F33" s="322"/>
       <c r="G33" s="67">
         <v>10</v>
       </c>
@@ -26009,7 +26009,7 @@
       <c r="E34" s="86" t="s">
         <v>319</v>
       </c>
-      <c r="F34" s="321"/>
+      <c r="F34" s="322"/>
       <c r="G34" s="67">
         <v>5</v>
       </c>
@@ -26083,7 +26083,7 @@
       <c r="E36" s="87" t="s">
         <v>319</v>
       </c>
-      <c r="F36" s="321"/>
+      <c r="F36" s="322"/>
       <c r="G36" s="67">
         <v>70</v>
       </c>
@@ -26119,7 +26119,7 @@
       <c r="E37" s="88" t="s">
         <v>320</v>
       </c>
-      <c r="F37" s="322"/>
+      <c r="F37" s="321"/>
       <c r="G37" s="68">
         <v>10</v>
       </c>
@@ -26207,7 +26207,7 @@
       <c r="E40" s="90" t="s">
         <v>317</v>
       </c>
-      <c r="F40" s="321"/>
+      <c r="F40" s="322"/>
       <c r="G40" s="67">
         <v>50</v>
       </c>
@@ -26243,7 +26243,7 @@
       <c r="E41" s="90" t="s">
         <v>317</v>
       </c>
-      <c r="F41" s="321"/>
+      <c r="F41" s="322"/>
       <c r="G41" s="67">
         <v>20</v>
       </c>
@@ -26279,7 +26279,7 @@
       <c r="E42" s="90" t="s">
         <v>318</v>
       </c>
-      <c r="F42" s="321"/>
+      <c r="F42" s="322"/>
       <c r="G42" s="67">
         <v>10</v>
       </c>
@@ -26353,7 +26353,7 @@
       <c r="E44" s="91" t="s">
         <v>318</v>
       </c>
-      <c r="F44" s="321"/>
+      <c r="F44" s="322"/>
       <c r="G44" s="67">
         <v>10</v>
       </c>
@@ -26389,7 +26389,7 @@
       <c r="E45" s="91" t="s">
         <v>319</v>
       </c>
-      <c r="F45" s="321"/>
+      <c r="F45" s="322"/>
       <c r="G45" s="67">
         <v>30</v>
       </c>
@@ -26425,7 +26425,7 @@
       <c r="E46" s="92" t="s">
         <v>320</v>
       </c>
-      <c r="F46" s="322"/>
+      <c r="F46" s="321"/>
       <c r="G46" s="68">
         <v>10</v>
       </c>
@@ -26513,7 +26513,7 @@
       <c r="E49" s="94" t="s">
         <v>318</v>
       </c>
-      <c r="F49" s="321"/>
+      <c r="F49" s="322"/>
       <c r="G49" s="67">
         <v>20</v>
       </c>
@@ -26549,7 +26549,7 @@
       <c r="E50" s="94" t="s">
         <v>318</v>
       </c>
-      <c r="F50" s="321"/>
+      <c r="F50" s="322"/>
       <c r="G50" s="67">
         <v>10</v>
       </c>
@@ -26675,7 +26675,7 @@
       <c r="E54" s="96" t="s">
         <v>317</v>
       </c>
-      <c r="F54" s="321"/>
+      <c r="F54" s="322"/>
       <c r="G54" s="67">
         <v>20</v>
       </c>
@@ -26711,7 +26711,7 @@
       <c r="E55" s="96" t="s">
         <v>318</v>
       </c>
-      <c r="F55" s="321"/>
+      <c r="F55" s="322"/>
       <c r="G55" s="67">
         <v>10</v>
       </c>
@@ -26785,7 +26785,7 @@
       <c r="E57" s="97" t="s">
         <v>319</v>
       </c>
-      <c r="F57" s="321"/>
+      <c r="F57" s="322"/>
       <c r="G57" s="67">
         <v>15</v>
       </c>
@@ -26821,7 +26821,7 @@
       <c r="E58" s="98" t="s">
         <v>319</v>
       </c>
-      <c r="F58" s="322"/>
+      <c r="F58" s="321"/>
       <c r="G58" s="68">
         <v>5</v>
       </c>
@@ -26909,7 +26909,7 @@
       <c r="E61" s="100" t="s">
         <v>319</v>
       </c>
-      <c r="F61" s="321"/>
+      <c r="F61" s="322"/>
       <c r="G61" s="67">
         <v>20</v>
       </c>
@@ -26945,7 +26945,7 @@
       <c r="E62" s="100" t="s">
         <v>319</v>
       </c>
-      <c r="F62" s="321"/>
+      <c r="F62" s="322"/>
       <c r="G62" s="67">
         <v>20</v>
       </c>
@@ -26981,7 +26981,7 @@
       <c r="E63" s="100" t="s">
         <v>320</v>
       </c>
-      <c r="F63" s="321"/>
+      <c r="F63" s="322"/>
       <c r="G63" s="67">
         <v>15</v>
       </c>
@@ -27017,7 +27017,7 @@
       <c r="E64" s="100" t="s">
         <v>320</v>
       </c>
-      <c r="F64" s="321"/>
+      <c r="F64" s="322"/>
       <c r="G64" s="67">
         <v>15</v>
       </c>
@@ -27053,7 +27053,7 @@
       <c r="E65" s="100" t="s">
         <v>320</v>
       </c>
-      <c r="F65" s="321"/>
+      <c r="F65" s="322"/>
       <c r="G65" s="67">
         <v>10</v>
       </c>
@@ -27127,7 +27127,7 @@
       <c r="E67" s="101" t="s">
         <v>321</v>
       </c>
-      <c r="F67" s="322"/>
+      <c r="F67" s="321"/>
       <c r="G67" s="68">
         <v>20</v>
       </c>
@@ -27215,7 +27215,7 @@
       <c r="E70" s="103" t="s">
         <v>318</v>
       </c>
-      <c r="F70" s="321"/>
+      <c r="F70" s="322"/>
       <c r="G70" s="67">
         <v>35</v>
       </c>
@@ -27251,7 +27251,7 @@
       <c r="E71" s="103" t="s">
         <v>318</v>
       </c>
-      <c r="F71" s="321"/>
+      <c r="F71" s="322"/>
       <c r="G71" s="67">
         <v>20</v>
       </c>
@@ -27287,7 +27287,7 @@
       <c r="E72" s="103" t="s">
         <v>319</v>
       </c>
-      <c r="F72" s="321"/>
+      <c r="F72" s="322"/>
       <c r="G72" s="67">
         <v>10</v>
       </c>
@@ -27361,7 +27361,7 @@
       <c r="E74" s="104" t="s">
         <v>320</v>
       </c>
-      <c r="F74" s="322"/>
+      <c r="F74" s="321"/>
       <c r="G74" s="68">
         <v>75</v>
       </c>
@@ -27411,7 +27411,7 @@
       <c r="E76" s="105" t="s">
         <v>320</v>
       </c>
-      <c r="F76" s="321">
+      <c r="F76" s="322">
         <v>60</v>
       </c>
       <c r="G76" s="67">
@@ -27449,7 +27449,7 @@
       <c r="E77" s="105" t="s">
         <v>320</v>
       </c>
-      <c r="F77" s="321"/>
+      <c r="F77" s="322"/>
       <c r="G77" s="67">
         <v>75</v>
       </c>
@@ -27523,7 +27523,7 @@
       <c r="E79" s="106" t="s">
         <v>321</v>
       </c>
-      <c r="F79" s="322"/>
+      <c r="F79" s="321"/>
       <c r="G79" s="68">
         <v>75</v>
       </c>
@@ -27658,15 +27658,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="F73:F74"/>
-    <mergeCell ref="F76:F77"/>
-    <mergeCell ref="F78:F79"/>
-    <mergeCell ref="F48:F50"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="F56:F58"/>
-    <mergeCell ref="F60:F65"/>
-    <mergeCell ref="F66:F67"/>
-    <mergeCell ref="F69:F72"/>
     <mergeCell ref="F43:F46"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="H1:L1"/>
@@ -27679,6 +27670,15 @@
     <mergeCell ref="F30:F34"/>
     <mergeCell ref="F35:F37"/>
     <mergeCell ref="F39:F42"/>
+    <mergeCell ref="F73:F74"/>
+    <mergeCell ref="F76:F77"/>
+    <mergeCell ref="F78:F79"/>
+    <mergeCell ref="F48:F50"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="F56:F58"/>
+    <mergeCell ref="F60:F65"/>
+    <mergeCell ref="F66:F67"/>
+    <mergeCell ref="F69:F72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>